<commit_message>
🔄 Actualización automática del mapa (2025-07-18 07:34:36)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P396"/>
+  <dimension ref="A1:P400"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30313,6 +30313,310 @@
         </is>
       </c>
       <c r="P396" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>6437</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>MILLER 4590</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>808400306</t>
+        </is>
+      </c>
+      <c r="F397" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G397" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H397" t="inlineStr">
+        <is>
+          <t>Columna corroida</t>
+        </is>
+      </c>
+      <c r="I397" t="n">
+        <v>1</v>
+      </c>
+      <c r="J397" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K397" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L397" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M397" t="n">
+        <v>-58.495482</v>
+      </c>
+      <c r="N397" t="n">
+        <v>-34.552614</v>
+      </c>
+      <c r="O397" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P397" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>6447</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>CIUDAD DE LA PAZ 1535</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>808400333</t>
+        </is>
+      </c>
+      <c r="F398" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G398" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H398" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I398" t="n">
+        <v>1</v>
+      </c>
+      <c r="J398" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K398" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L398" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M398" t="n">
+        <v>-58.453124</v>
+      </c>
+      <c r="N398" t="n">
+        <v>-34.567382</v>
+      </c>
+      <c r="O398" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P398" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>-519</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>Vilela 2687</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>808400334</t>
+        </is>
+      </c>
+      <c r="F399" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G399" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H399" t="inlineStr">
+        <is>
+          <t>CAmbiar columna 114 picada en base</t>
+        </is>
+      </c>
+      <c r="I399" t="n">
+        <v>1</v>
+      </c>
+      <c r="J399" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K399" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L399" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M399" t="n">
+        <v>-58.472968</v>
+      </c>
+      <c r="N399" t="n">
+        <v>-34.546898</v>
+      </c>
+      <c r="O399" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P399" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>-520</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>Pedraza Manuela 4101</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>808400353</t>
+        </is>
+      </c>
+      <c r="F400" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G400" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Podrida en la base </t>
+        </is>
+      </c>
+      <c r="I400" t="n">
+        <v>1</v>
+      </c>
+      <c r="J400" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K400" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L400" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M400" t="n">
+        <v>-58.481569</v>
+      </c>
+      <c r="N400" t="n">
+        <v>-34.559853</v>
+      </c>
+      <c r="O400" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P400" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>
@@ -42563,7 +42867,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -46660,6 +46964,310 @@
         </is>
       </c>
       <c r="P54" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>6437</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>MILLER 4590</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>808400306</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Columna corroida</t>
+        </is>
+      </c>
+      <c r="I55" t="n">
+        <v>1</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M55" t="n">
+        <v>-58.495482</v>
+      </c>
+      <c r="N55" t="n">
+        <v>-34.552614</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>6447</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>CIUDAD DE LA PAZ 1535</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>808400333</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I56" t="n">
+        <v>1</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M56" t="n">
+        <v>-58.453124</v>
+      </c>
+      <c r="N56" t="n">
+        <v>-34.567382</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>-519</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Vilela 2687</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>808400334</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>CAmbiar columna 114 picada en base</t>
+        </is>
+      </c>
+      <c r="I57" t="n">
+        <v>1</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M57" t="n">
+        <v>-58.472968</v>
+      </c>
+      <c r="N57" t="n">
+        <v>-34.546898</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>-520</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>7/17/2025</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Pedraza Manuela 4101</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>808400353</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Podrida en la base </t>
+        </is>
+      </c>
+      <c r="I58" t="n">
+        <v>1</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M58" t="n">
+        <v>-58.481569</v>
+      </c>
+      <c r="N58" t="n">
+        <v>-34.559853</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-24 06:58:24)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -28981,7 +28981,7 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>-526</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
@@ -28991,22 +28991,18 @@
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>Moldes 1813</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D378" t="inlineStr">
         <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E378" t="inlineStr">
-        <is>
-          <t>808488825</t>
-        </is>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E378" t="inlineStr"/>
       <c r="F378" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>Optical Power</t>
         </is>
       </c>
       <c r="G378" t="inlineStr">
@@ -29016,7 +29012,7 @@
       </c>
       <c r="H378" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I378" t="n">
@@ -29038,19 +29034,19 @@
         </is>
       </c>
       <c r="M378" t="n">
-        <v>-58.457145</v>
+        <v>-58.384097</v>
       </c>
       <c r="N378" t="n">
-        <v>-34.56629</v>
+        <v>-34.598913</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P378" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
@@ -34238,7 +34234,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P88"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40919,6 +40915,78 @@
         </is>
       </c>
       <c r="P88" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>-529</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>7/23/2025</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Libertad 820</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>1</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>-58.384097</v>
+      </c>
+      <c r="N89" t="n">
+        <v>-34.598913</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Recoleta</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
@@ -40935,7 +41003,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P59"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -45336,82 +45404,6 @@
         </is>
       </c>
       <c r="P58" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>-526</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>7/23/2025</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Moldes 1813</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>808488825</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I59" t="n">
-        <v>1</v>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M59" t="n">
-        <v>-58.457145</v>
-      </c>
-      <c r="N59" t="n">
-        <v>-34.56629</v>
-      </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>Colegiales</t>
-        </is>
-      </c>
-      <c r="P59" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-29 09:07:59)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -14,7 +14,6 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Propio" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AYKO" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="INCO" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sin_Asignar" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -28722,7 +28721,7 @@
       </c>
       <c r="F374" t="inlineStr">
         <is>
-          <t>Sin Asignar</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G374" t="inlineStr">
@@ -28732,7 +28731,7 @@
       </c>
       <c r="H374" t="inlineStr">
         <is>
-          <t>Columna partida enganchada en tendido con riesgo de caida urgente</t>
+          <t>Traspasar red y desmontar</t>
         </is>
       </c>
       <c r="I374" t="n">
@@ -29309,7 +29308,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P79"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34918,7 +34917,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6522</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -34928,7 +34927,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 384</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -34938,7 +34937,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808571978</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -34953,7 +34952,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspasar red y desmontar</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -34975,10 +34974,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.466359</v>
+        <v>-58.466995</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.625966</v>
+        <v>-34.626426</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -34994,7 +34993,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -35004,17 +35003,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -35051,14 +35050,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.433295</v>
+        <v>-58.466359</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.574305</v>
+        <v>-34.625966</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -35070,7 +35069,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -35080,17 +35079,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -35127,10 +35126,10 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.447943</v>
+        <v>-58.433295</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.580719</v>
+        <v>-34.574305</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -35146,7 +35145,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -35156,17 +35155,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -35203,10 +35202,10 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.437823</v>
+        <v>-58.447943</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.600094</v>
+        <v>-34.580719</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -35222,74 +35221,150 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
+          <t>-532</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>7/28/2025</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Av Corrientes 5143</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>808571983</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>1</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M79" t="n">
+        <v>-58.437823</v>
+      </c>
+      <c r="N79" t="n">
+        <v>-34.600094</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
           <t>-533</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="B80" t="inlineStr">
         <is>
           <t>7/28/2025</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
+      <c r="C80" t="inlineStr">
         <is>
           <t>Bonpland 2233</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
+      <c r="D80" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
+      <c r="E80" t="inlineStr">
         <is>
           <t>808571985</t>
         </is>
       </c>
-      <c r="F79" t="inlineStr">
+      <c r="F80" t="inlineStr">
         <is>
           <t>PEBCOM</t>
         </is>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
         <is>
           <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
-      <c r="I79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L79" t="inlineStr">
+      <c r="I80" t="n">
+        <v>1</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
         <is>
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M79" t="n">
+      <c r="M80" t="n">
         <v>-58.43258</v>
       </c>
-      <c r="N79" t="n">
+      <c r="N80" t="n">
         <v>-34.579265</v>
       </c>
-      <c r="O79" t="inlineStr">
+      <c r="O80" t="inlineStr">
         <is>
           <t>Palermo</t>
         </is>
       </c>
-      <c r="P79" t="inlineStr">
+      <c r="P80" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
@@ -58607,181 +58682,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:P2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Caso</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>F. De Reclamo</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Direccion</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Comuna</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>OT</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Proveedor Asignado</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Estado</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Observaciones</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Attachments</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Tipo de tarea</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Equipo</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Tipo de Elemento</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Coordenada_X</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Coordenada_Y</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Operacion</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Zona</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>6522</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>7/28/2025</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 384</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>808571978</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Sin Asignar</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Columna partida enganchada en tendido con riesgo de caida urgente</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>-58.466995</v>
-      </c>
-      <c r="N2" t="n">
-        <v>-34.626426</v>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-29 12:28:02)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -29246,7 +29246,11 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E381" t="inlineStr"/>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>ICD30238810</t>
+        </is>
+      </c>
       <c r="F381" t="inlineStr">
         <is>
           <t>NEW</t>
@@ -47649,7 +47653,11 @@
           <t>4</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr"/>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>ICD30238810</t>
+        </is>
+      </c>
       <c r="F68" t="inlineStr">
         <is>
           <t>NEW</t>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-02 07:27:31)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P372"/>
+  <dimension ref="A1:P375"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17414,7 +17414,7 @@
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G225" t="inlineStr">
@@ -28278,7 +28278,7 @@
       </c>
       <c r="F368" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G368" t="inlineStr">
@@ -28627,6 +28627,230 @@
       <c r="P372" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>-541</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>8/1/2025</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>AYACUCHO 241</t>
+        </is>
+      </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>808663880</t>
+        </is>
+      </c>
+      <c r="F373" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G373" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H373" t="inlineStr">
+        <is>
+          <t>Colocar columna para pedir traspaso de nodo</t>
+        </is>
+      </c>
+      <c r="I373" t="n">
+        <v>1</v>
+      </c>
+      <c r="J373" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K373" t="inlineStr">
+        <is>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L373" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M373" t="n">
+        <v>-58.395015</v>
+      </c>
+      <c r="N373" t="n">
+        <v>-34.606755</v>
+      </c>
+      <c r="O373" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P373" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>-542</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>8/1/2025</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>Cramer 2141</t>
+        </is>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>808663881</t>
+        </is>
+      </c>
+      <c r="F374" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G374" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H374" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+        </is>
+      </c>
+      <c r="I374" t="n">
+        <v>1</v>
+      </c>
+      <c r="J374" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K374" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L374" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M374" t="n">
+        <v>-58.461582</v>
+      </c>
+      <c r="N374" t="n">
+        <v>-34.564296</v>
+      </c>
+      <c r="O374" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P374" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>-543</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>8/1/2025</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>Pedro Ignacio Rivera 3258</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E375" t="inlineStr"/>
+      <c r="F375" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G375" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H375" t="inlineStr">
+        <is>
+          <t>Desmontar poste en desuso</t>
+        </is>
+      </c>
+      <c r="I375" t="n">
+        <v>1</v>
+      </c>
+      <c r="J375" t="inlineStr">
+        <is>
+          <t>Desmonte</t>
+        </is>
+      </c>
+      <c r="K375" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L375" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M375" t="n">
+        <v>-58.46967</v>
+      </c>
+      <c r="N375" t="n">
+        <v>-34.561676</v>
+      </c>
+      <c r="O375" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P375" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
@@ -28641,7 +28865,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P80"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34700,6 +34924,82 @@
       <c r="P80" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>-541</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>8/1/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>AYACUCHO 241</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>808663880</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Colocar columna para pedir traspaso de nodo</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>-58.395015</v>
+      </c>
+      <c r="N81" t="n">
+        <v>-34.606755</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
@@ -41719,7 +42019,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P64"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44304,17 +44604,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5826</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3180</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -44324,7 +44624,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>806926466</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -44339,7 +44639,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Columna (metal) inclinada</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -44347,7 +44647,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -44361,14 +44661,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.513552</v>
+        <v>-58.488252</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.579829</v>
+        <v>-34.553391</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -44380,7 +44680,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5825</t>
+          <t>5826</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -44390,7 +44690,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>PAZ, GRAL. AV. 5602</t>
+          <t>ALBARELLOS AV. 3180</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -44400,7 +44700,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>806926472</t>
+          <t>806926466</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -44415,7 +44715,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
+          <t>Columna (metal) inclinada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -44423,7 +44723,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -44437,10 +44737,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.513685</v>
+        <v>-58.513552</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.579838</v>
+        <v>-34.579829</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -44456,17 +44756,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5875</t>
+          <t>5825</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>MONROE 4096</t>
+          <t>PAZ, GRAL. AV. 5602</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -44476,7 +44776,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>806975680</t>
+          <t>806926472</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -44491,7 +44791,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>reparar rienda cortada - ver foto no es la misma que albarellos</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -44499,7 +44799,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -44509,18 +44809,18 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.476106</v>
+        <v>-58.513685</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.568373</v>
+        <v>-34.579838</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -44532,27 +44832,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>5875</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>O'Higgins 4379</t>
+          <t>MONROE 4096</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807044192</t>
+          <t>806975680</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -44567,7 +44867,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -44575,7 +44875,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -44585,18 +44885,18 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.468425</v>
+        <v>-58.476106</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.54124</v>
+        <v>-34.568373</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -44608,27 +44908,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6020</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>RAVIGNANI, EMILIO, DR. 2036</t>
+          <t>O'Higgins 4379</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807215465</t>
+          <t>807044192</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -44643,7 +44943,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Poste </t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -44651,7 +44951,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -44661,50 +44961,50 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.436298</v>
+        <v>-58.468425</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.578972</v>
+        <v>-34.54124</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6144</t>
+          <t>6020</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/11/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>TURIN 2990</t>
+          <t>RAVIGNANI, EMILIO, DR. 2036</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807458282</t>
+          <t>807215465</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -44741,26 +45041,26 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.480925</v>
+        <v>-58.436298</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.585471</v>
+        <v>-34.578972</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6143</t>
+          <t>6144</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -44770,7 +45070,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
+          <t>TURIN 2990</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -44780,7 +45080,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807458296</t>
+          <t>807458282</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -44817,10 +45117,10 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.495071</v>
+        <v>-58.480925</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.593122</v>
+        <v>-34.585471</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -44836,7 +45136,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6141</t>
+          <t>6143</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -44846,17 +45146,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>EL PAMPERO 2618</t>
+          <t>SOLANO LOPEZ, F., MARISCAL 2845</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807458310</t>
+          <t>807458296</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -44893,10 +45193,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.481942</v>
+        <v>-58.495071</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.602989</v>
+        <v>-34.593122</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -44912,17 +45212,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-478</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6/15/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Chivilcoy 4875</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -44932,7 +45232,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807508509</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -44947,7 +45247,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Poste podrido</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -44965,14 +45265,14 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.517389</v>
+        <v>-58.481942</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.593541</v>
+        <v>-34.602989</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -44988,27 +45288,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6171</t>
+          <t>-478</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/15/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>CABELLO 3486</t>
+          <t>Chivilcoy 4875</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807658640</t>
+          <t>807508509</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -45023,7 +45323,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Columna inclinada evaluar con inspector un corrimiento</t>
+          <t>Poste podrido</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -45041,40 +45341,40 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.409579</v>
+        <v>-58.517389</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.581134</v>
+        <v>-34.593541</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6230</t>
+          <t>6171</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Santa maria de oro	2722</t>
+          <t>CABELLO 3486</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -45084,7 +45384,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807763066</t>
+          <t>807658640</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -45099,7 +45399,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada evaluar con inspector un corrimiento</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -45121,10 +45421,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.422315</v>
+        <v>-58.409579</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.576988</v>
+        <v>-34.581134</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -45140,7 +45440,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>6230</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -45150,7 +45450,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 275</t>
+          <t>Santa maria de oro	2722</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -45160,7 +45460,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807763070</t>
+          <t>807763066</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -45175,7 +45475,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -45193,14 +45493,14 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.441049</v>
+        <v>-58.422315</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.574625</v>
+        <v>-34.576988</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -45216,7 +45516,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6235</t>
+          <t>6231</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -45226,17 +45526,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>HUERGO 389</t>
+          <t>Ciudad de la Paz 275</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807763078</t>
+          <t>807763070</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -45251,7 +45551,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar o cambiar</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -45269,14 +45569,14 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.432722</v>
+        <v>-58.441049</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.572371</v>
+        <v>-34.574625</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -45292,27 +45592,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6295</t>
+          <t>6235</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>SOLER 6017</t>
+          <t>HUERGO 389</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807851636</t>
+          <t>807763078</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -45349,10 +45649,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.436808</v>
+        <v>-58.432722</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.577464</v>
+        <v>-34.572371</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -45368,17 +45668,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6332</t>
+          <t>6295</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ARAOZ 2560</t>
+          <t>SOLER 6017</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -45388,7 +45688,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807965818</t>
+          <t>807851636</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -45425,10 +45725,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.414507</v>
+        <v>-58.436808</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.585377</v>
+        <v>-34.577464</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -45444,27 +45744,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>6332</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>MOLDES 3730</t>
+          <t>ARAOZ 2560</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808099415</t>
+          <t>807965818</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -45479,7 +45779,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -45487,7 +45787,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -45497,50 +45797,50 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.47192</v>
+        <v>-58.414507</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.549398</v>
+        <v>-34.585377</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-503</t>
+          <t>6363</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/10/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Salguero 842</t>
+          <t>MOLDES 3730</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808148673</t>
+          <t>808099415</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -45555,7 +45855,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Cambiar columna picada en la base</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -45563,7 +45863,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -45573,30 +45873,30 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.419166</v>
+        <v>-58.47192</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.600265</v>
+        <v>-34.549398</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6506</t>
+          <t>-503</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -45606,17 +45906,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Ohiggins 1611</t>
+          <t>Salguero 842</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808148679</t>
+          <t>808148673</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -45631,7 +45931,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Cambiar columna picada en la base</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -45644,7 +45944,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -45653,46 +45953,46 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.448993</v>
+        <v>-58.419166</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.564383</v>
+        <v>-34.600265</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6437</t>
+          <t>6506</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/17/2025</t>
+          <t>7/10/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>MILLER 4590</t>
+          <t>Ohiggins 1611</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808400306</t>
+          <t>808148679</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -45707,7 +46007,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Columna corroida</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -45720,7 +46020,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -45729,14 +46029,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.495482</v>
+        <v>-58.448993</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.552614</v>
+        <v>-34.564383</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -45748,7 +46048,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6447</t>
+          <t>6437</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -45758,17 +46058,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1535</t>
+          <t>MILLER 4590</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808400333</t>
+          <t>808400306</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -45783,7 +46083,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -45805,14 +46105,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.453124</v>
+        <v>-58.495482</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.567382</v>
+        <v>-34.552614</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -45824,7 +46124,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-519</t>
+          <t>6447</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -45834,17 +46134,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Vilela 2687</t>
+          <t>CIUDAD DE LA PAZ 1535</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808400334</t>
+          <t>808400333</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -45859,7 +46159,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>CAmbiar columna 114 picada en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -45881,14 +46181,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.472968</v>
+        <v>-58.453124</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.546898</v>
+        <v>-34.567382</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -45900,7 +46200,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6538</t>
+          <t>-519</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -45910,7 +46210,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Pedraza Manuela 4101</t>
+          <t>Vilela 2687</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -45920,7 +46220,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808400353</t>
+          <t>808400334</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -45935,7 +46235,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Podrida en la base </t>
+          <t>CAmbiar columna 114 picada en base</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -45957,10 +46257,10 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.481569</v>
+        <v>-58.472968</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.559853</v>
+        <v>-34.546898</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -45976,27 +46276,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>6538</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/22/2025</t>
+          <t>7/17/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>Pedraza Manuela 4101</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808480549</t>
+          <t>808400353</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -46011,7 +46311,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Corroida en base para recambio</t>
+          <t xml:space="preserve">Podrida en la base </t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -46033,14 +46333,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.457492</v>
+        <v>-58.481569</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.579336</v>
+        <v>-34.559853</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -46052,27 +46352,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6484</t>
+          <t>-525</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/22/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>URIARTE 2396</t>
+          <t>Zabala 3567</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808509373</t>
+          <t>808480549</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -46087,7 +46387,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Corroida en base para recambio</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -46109,46 +46409,46 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.423934</v>
+        <v>-58.457492</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.581562</v>
+        <v>-34.579336</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6502</t>
+          <t>6484</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1511</t>
+          <t>URIARTE 2396</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808571972</t>
+          <t>808509373</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -46185,26 +46485,26 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.452907</v>
+        <v>-58.423934</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.567508</v>
+        <v>-34.581562</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6504</t>
+          <t>6502</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -46214,7 +46514,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 1278</t>
+          <t>CIUDAD DE LA PAZ 1511</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -46224,7 +46524,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808571974</t>
+          <t>808571972</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -46239,7 +46539,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -46261,10 +46561,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.450753</v>
+        <v>-58.452907</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.5688</v>
+        <v>-34.567508</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -46280,27 +46580,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6512</t>
+          <t>6504</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>GASCON 1195</t>
+          <t>CIUDAD DE LA PAZ 1278</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808571975</t>
+          <t>808571974</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -46315,7 +46615,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -46337,26 +46637,26 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.423127</v>
+        <v>-58.450753</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.596476</v>
+        <v>-34.5688</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6513</t>
+          <t>6512</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -46366,7 +46666,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>DORREGO 1925</t>
+          <t>GASCON 1195</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -46376,7 +46676,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808571976</t>
+          <t>808571975</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -46413,10 +46713,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.441281</v>
+        <v>-58.423127</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.579867</v>
+        <v>-34.596476</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -46432,7 +46732,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6519</t>
+          <t>6513</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -46442,7 +46742,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>SALGUERO, JERONIMO 2874</t>
+          <t>DORREGO 1925</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -46452,7 +46752,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808571977</t>
+          <t>808571976</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -46467,7 +46767,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -46475,7 +46775,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -46485,14 +46785,14 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.407256</v>
+        <v>-58.441281</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.578976</v>
+        <v>-34.579867</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -46508,76 +46808,300 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
+          <t>6519</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>7/28/2025</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>SALGUERO, JERONIMO 2874</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>808571977</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Reparar rienda</t>
+        </is>
+      </c>
+      <c r="I64" t="n">
+        <v>1</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>Tensor</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M64" t="n">
+        <v>-58.407256</v>
+      </c>
+      <c r="N64" t="n">
+        <v>-34.578976</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>-536</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>7/29/2025</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Olof palme 4142</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ICD30249764 </t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Aplomar o desmontar poste</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>1</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Desmonte</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M65" t="n">
+        <v>-58.488239</v>
+      </c>
+      <c r="N65" t="n">
+        <v>-34.55341</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
           <t>-538</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
+      <c r="B66" t="inlineStr">
         <is>
           <t>7/31/2025</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="C66" t="inlineStr">
         <is>
           <t>Malabia 964</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
+      <c r="D66" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
+      <c r="E66" t="inlineStr">
         <is>
           <t>808609237</t>
         </is>
       </c>
-      <c r="F64" t="inlineStr">
+      <c r="F66" t="inlineStr">
         <is>
           <t>NEW</t>
         </is>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
         <is>
           <t>Cambiar poste mal estado por PRFV</t>
         </is>
       </c>
-      <c r="I64" t="n">
-        <v>1</v>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L64" t="inlineStr">
+      <c r="I66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
         <is>
           <t>Poste</t>
         </is>
       </c>
-      <c r="M64" t="n">
+      <c r="M66" t="n">
         <v>-58.433634</v>
       </c>
-      <c r="N64" t="n">
+      <c r="N66" t="n">
         <v>-34.595018</v>
       </c>
-      <c r="O64" t="inlineStr">
+      <c r="O66" t="inlineStr">
         <is>
           <t>Palermo</t>
         </is>
       </c>
-      <c r="P64" t="inlineStr">
+      <c r="P66" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>-543</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>8/1/2025</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Pedro Ignacio Rivera 3258</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Desmontar poste en desuso</t>
+        </is>
+      </c>
+      <c r="I67" t="n">
+        <v>1</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>Desmonte</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M67" t="n">
+        <v>-58.46967</v>
+      </c>
+      <c r="N67" t="n">
+        <v>-34.561676</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
@@ -46921,7 +47445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P88"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -51558,7 +52082,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -51568,7 +52092,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -51578,7 +52102,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -51593,7 +52117,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -51601,7 +52125,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -51615,10 +52139,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.488252</v>
+        <v>-58.470837</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.553391</v>
+        <v>-34.545751</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -51634,7 +52158,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -51644,7 +52168,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -51654,7 +52178,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -51669,7 +52193,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -51682,19 +52206,19 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.470837</v>
+        <v>-58.472267</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.545751</v>
+        <v>-34.551163</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -51710,27 +52234,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -51745,7 +52269,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -51753,12 +52277,12 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L64" t="inlineStr">
@@ -51767,10 +52291,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.472267</v>
+        <v>-58.464144</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.551163</v>
+        <v>-34.541832</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -51786,7 +52310,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -51796,17 +52320,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -51821,7 +52345,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -51843,26 +52367,26 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.464144</v>
+        <v>-58.434761</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.541832</v>
+        <v>-34.598381</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -51872,17 +52396,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -51897,7 +52421,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -51915,30 +52439,30 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.434761</v>
+        <v>-58.464177</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.598381</v>
+        <v>-34.558239</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -51948,17 +52472,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -51973,7 +52497,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -51991,50 +52515,50 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.464177</v>
+        <v>-58.412302</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.558239</v>
+        <v>-34.59301</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -52049,11 +52573,11 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -52071,46 +52595,46 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.412302</v>
+        <v>-58.485056</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.59301</v>
+        <v>-34.555059</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/22/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>Cucha Cucha 2918</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -52125,15 +52649,15 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -52147,14 +52671,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.485056</v>
+        <v>-58.469783</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.555059</v>
+        <v>-34.599214</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -52166,27 +52690,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>5/22/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Cucha Cucha 2918</t>
+          <t>Martin Grandoli 5761</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t xml:space="preserve">ICD30261461 </t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -52201,7 +52725,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -52209,7 +52733,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -52219,30 +52743,30 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.469783</v>
+        <v>-58.487144</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.599214</v>
+        <v>-34.669078</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>807044233</t>
+          <t>6496</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -52252,17 +52776,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Martin Grandoli 5761</t>
+          <t>Moldes 2327</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30261461 </t>
+          <t>807044059</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -52277,7 +52801,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -52285,7 +52809,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -52295,50 +52819,50 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.487144</v>
+        <v>-58.461172</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.669078</v>
+        <v>-34.561608</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6496</t>
+          <t>-480</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Moldes 2327</t>
+          <t>Arias 4384</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>807044059</t>
+          <t>807537909</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -52353,7 +52877,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -52375,10 +52899,10 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.461172</v>
+        <v>-58.49147</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.561608</v>
+        <v>-34.55031</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -52394,27 +52918,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Arias 4384</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>807537909</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -52427,11 +52951,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>Inclinada</t>
-        </is>
-      </c>
+      <c r="H73" t="inlineStr"/>
       <c r="I73" t="n">
         <v>1</v>
       </c>
@@ -52451,36 +52971,36 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.49147</v>
+        <v>-58.405761</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.55031</v>
+        <v>-34.582476</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -52490,7 +53010,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -52503,7 +53023,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H74" t="inlineStr"/>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I74" t="n">
         <v>1</v>
       </c>
@@ -52523,14 +53047,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.405761</v>
+        <v>-58.432241</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.582476</v>
+        <v>-34.56642</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -52542,7 +53066,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -52552,7 +53076,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -52562,7 +53086,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -52577,7 +53101,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -52599,10 +53123,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.432241</v>
+        <v>-58.417348</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.56642</v>
+        <v>-34.595467</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -52618,27 +53142,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -52653,7 +53177,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -52671,18 +53195,18 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.417348</v>
+        <v>-58.472311</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.595467</v>
+        <v>-34.654867</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -52694,7 +53218,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>6239</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -52704,17 +53228,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>PALPA 2964</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807763098</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -52729,7 +53253,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -52747,30 +53271,30 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.472311</v>
+        <v>-58.450113</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.654867</v>
+        <v>-34.574534</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6239</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -52780,17 +53304,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>PALPA 2964</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>807763098</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -52805,7 +53329,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -52823,18 +53347,18 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.450113</v>
+        <v>-58.484729</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.574534</v>
+        <v>-34.574614</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -52846,27 +53370,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>-491</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>3 de Febrero 2171</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807789702</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -52881,7 +53405,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Columna 114 propia picada en base con NAP</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -52899,18 +53423,18 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.484729</v>
+        <v>-58.452636</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.574614</v>
+        <v>-34.558607</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -52922,27 +53446,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>-491</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>3 de Febrero 2171</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>807789702</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -52957,7 +53481,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Columna 114 propia picada en base con NAP</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -52965,7 +53489,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -52975,18 +53499,18 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.452636</v>
+        <v>-58.510247</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.558607</v>
+        <v>-34.645038</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -52998,7 +53522,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6410</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -53008,17 +53532,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>BEAUCHEF 421</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>808373658</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -53033,7 +53557,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -53041,7 +53565,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -53051,50 +53575,50 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.510247</v>
+        <v>-58.433724</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.645038</v>
+        <v>-34.621643</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6410</t>
+          <t>-518</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>BEAUCHEF 421</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808373658</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -53109,7 +53633,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -53131,46 +53655,46 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.433724</v>
+        <v>-58.483145</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.621643</v>
+        <v>-34.557043</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-518</t>
+          <t>6454</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/18/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t>HABANA 3382</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>808413466</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -53185,7 +53709,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -53207,14 +53731,14 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.483145</v>
+        <v>-58.505747</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.557043</v>
+        <v>-34.593173</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -53226,27 +53750,27 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>6454</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>7/18/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>HABANA 3382</t>
+          <t>Laferrere 6572</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808413466</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -53261,7 +53785,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -53283,14 +53807,14 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.505747</v>
+        <v>-58.496608</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.593173</v>
+        <v>-34.666371</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -53302,27 +53826,27 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6472</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Laferrere 6572</t>
+          <t>DUMONT, SANTOS 3744</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808509381</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -53337,7 +53861,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -53355,18 +53879,18 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.496608</v>
+        <v>-58.448576</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.666371</v>
+        <v>-34.585794</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -53378,27 +53902,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>6472</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>DUMONT, SANTOS 3744</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>808509381</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -53413,7 +53937,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -53421,7 +53945,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -53431,175 +53955,23 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.448576</v>
+        <v>-58.422229</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.585794</v>
+        <v>-34.573148</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>6497</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>7/25/2025</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>808533127</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>Inclinada</t>
-        </is>
-      </c>
-      <c r="I87" t="n">
-        <v>1</v>
-      </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M87" t="n">
-        <v>-58.422229</v>
-      </c>
-      <c r="N87" t="n">
-        <v>-34.573148</v>
-      </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P87" t="inlineStr">
-        <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>-536</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>7/29/2025</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>Olof palme 4142</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ICD30249764 </t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>Aplomar o desmontar poste</t>
-        </is>
-      </c>
-      <c r="I88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>Desmonte</t>
-        </is>
-      </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M88" t="n">
-        <v>-58.488239</v>
-      </c>
-      <c r="N88" t="n">
-        <v>-34.55341</v>
-      </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P88" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
         </is>
       </c>
     </row>
@@ -57127,7 +57499,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -57445,6 +57817,82 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>-542</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>8/1/2025</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cramer 2141</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>808663881</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>-58.461582</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-34.564296</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-02 14:08:54)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P375"/>
+  <dimension ref="A1:P376"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28851,6 +28851,82 @@
       <c r="P375" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>-544</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>8/2/2025</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>Vera 453</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>808669129</t>
+        </is>
+      </c>
+      <c r="F376" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G376" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H376" t="inlineStr">
+        <is>
+          <t>Columna corroída en base</t>
+        </is>
+      </c>
+      <c r="I376" t="n">
+        <v>1</v>
+      </c>
+      <c r="J376" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K376" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L376" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M376" t="n">
+        <v>-58.437239</v>
+      </c>
+      <c r="N376" t="n">
+        <v>-34.599438</v>
+      </c>
+      <c r="O376" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P376" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
@@ -57499,7 +57575,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -57893,6 +57969,82 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>-544</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>8/2/2025</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Vera 453</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>808669129</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Columna corroída en base</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>-58.437239</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-34.599438</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-07 14:26:40)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P375"/>
+  <dimension ref="A1:P376"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3108,7 +3108,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Retirar PRFV telecentro ya traspaso nodo</t>
+          <t>Telecentro ya traspaso su nodo solo falta desmontar el prfv que quedo</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -21904,7 +21904,7 @@
       </c>
       <c r="H284" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
         </is>
       </c>
       <c r="I284" t="n">
@@ -24377,7 +24377,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>-512</t>
+          <t>6580</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
@@ -24985,7 +24985,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>-518</t>
+          <t>6585</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -27189,7 +27189,7 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>-541</t>
+          <t>6578</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
@@ -27209,7 +27209,7 @@
       </c>
       <c r="E354" t="inlineStr">
         <is>
-          <t>808663880</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
@@ -27873,7 +27873,7 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>-545</t>
+          <t>6193</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
@@ -27883,22 +27883,22 @@
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>Jeronimo Salguero 3601</t>
+          <t>POLA 591</t>
         </is>
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E363" t="inlineStr">
         <is>
-          <t>808713766</t>
+          <t>808720861</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G363" t="inlineStr">
@@ -27908,11 +27908,11 @@
       </c>
       <c r="H363" t="inlineStr">
         <is>
-          <t>Chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I363" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J363" t="inlineStr">
         <is>
@@ -27930,26 +27930,26 @@
         </is>
       </c>
       <c r="M363" t="n">
-        <v>-58.400953</v>
+        <v>-58.507385</v>
       </c>
       <c r="N363" t="n">
-        <v>-34.572274</v>
+        <v>-34.644479</v>
       </c>
       <c r="O363" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P363" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>6193</t>
+          <t>6277</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
@@ -27959,17 +27959,17 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>POLA 591</t>
+          <t>SENILLOSA 323</t>
         </is>
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>808720861</t>
+          <t>808720859</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
@@ -27988,7 +27988,7 @@
         </is>
       </c>
       <c r="I364" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J364" t="inlineStr">
         <is>
@@ -28006,26 +28006,26 @@
         </is>
       </c>
       <c r="M364" t="n">
-        <v>-58.507385</v>
+        <v>-58.429726</v>
       </c>
       <c r="N364" t="n">
-        <v>-34.644479</v>
+        <v>-34.619969</v>
       </c>
       <c r="O364" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P364" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>6277</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
@@ -28035,17 +28035,17 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>SENILLOSA 323</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E365" t="inlineStr">
         <is>
-          <t>808720859</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
@@ -28060,7 +28060,7 @@
       </c>
       <c r="H365" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I365" t="n">
@@ -28082,26 +28082,26 @@
         </is>
       </c>
       <c r="M365" t="n">
-        <v>-58.429726</v>
+        <v>-58.473089</v>
       </c>
       <c r="N365" t="n">
-        <v>-34.619969</v>
+        <v>-34.625478</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P365" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -28111,7 +28111,7 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D366" t="inlineStr">
@@ -28121,12 +28121,12 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>INCO</t>
         </is>
       </c>
       <c r="G366" t="inlineStr">
@@ -28136,7 +28136,7 @@
       </c>
       <c r="H366" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I366" t="n">
@@ -28158,14 +28158,14 @@
         </is>
       </c>
       <c r="M366" t="n">
-        <v>-58.473089</v>
+        <v>-58.511732</v>
       </c>
       <c r="N366" t="n">
-        <v>-34.625478</v>
+        <v>-34.578688</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P366" t="inlineStr">
@@ -28177,17 +28177,17 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>-546</t>
+          <t>6498</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>Albarellos 3031</t>
+          <t>BUCARELLI 2087</t>
         </is>
       </c>
       <c r="D367" t="inlineStr">
@@ -28197,12 +28197,12 @@
       </c>
       <c r="E367" t="inlineStr">
         <is>
-          <t>808720857</t>
+          <t>808733908</t>
         </is>
       </c>
       <c r="F367" t="inlineStr">
         <is>
-          <t>INCO</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G367" t="inlineStr">
@@ -28212,7 +28212,7 @@
       </c>
       <c r="H367" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I367" t="n">
@@ -28234,10 +28234,10 @@
         </is>
       </c>
       <c r="M367" t="n">
-        <v>-58.511732</v>
+        <v>-58.485592</v>
       </c>
       <c r="N367" t="n">
-        <v>-34.578688</v>
+        <v>-34.578586</v>
       </c>
       <c r="O367" t="inlineStr">
         <is>
@@ -28253,7 +28253,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>6498</t>
+          <t>6469</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
@@ -28263,22 +28263,22 @@
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>BUCARELLI 2087</t>
+          <t>USPALLATA 3626</t>
         </is>
       </c>
       <c r="D368" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>808733908</t>
+          <t>808733910</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G368" t="inlineStr">
@@ -28288,7 +28288,7 @@
       </c>
       <c r="H368" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I368" t="n">
@@ -28296,7 +28296,7 @@
       </c>
       <c r="J368" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K368" t="inlineStr">
@@ -28310,26 +28310,26 @@
         </is>
       </c>
       <c r="M368" t="n">
-        <v>-58.485592</v>
+        <v>-58.414389</v>
       </c>
       <c r="N368" t="n">
-        <v>-34.578586</v>
+        <v>-34.641308</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P368" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>6469</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
@@ -28339,17 +28339,17 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>USPALLATA 3626</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E369" t="inlineStr">
         <is>
-          <t>808733910</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
@@ -28364,7 +28364,7 @@
       </c>
       <c r="H369" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I369" t="n">
@@ -28372,7 +28372,7 @@
       </c>
       <c r="J369" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K369" t="inlineStr">
@@ -28386,10 +28386,10 @@
         </is>
       </c>
       <c r="M369" t="n">
-        <v>-58.414389</v>
+        <v>-58.468841</v>
       </c>
       <c r="N369" t="n">
-        <v>-34.641308</v>
+        <v>-34.686635</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
@@ -28405,7 +28405,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
@@ -28415,17 +28415,17 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E370" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
@@ -28440,7 +28440,7 @@
       </c>
       <c r="H370" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I370" t="n">
@@ -28448,7 +28448,7 @@
       </c>
       <c r="J370" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K370" t="inlineStr">
@@ -28462,14 +28462,14 @@
         </is>
       </c>
       <c r="M370" t="n">
-        <v>-58.468841</v>
+        <v>-58.375684</v>
       </c>
       <c r="N370" t="n">
-        <v>-34.686635</v>
+        <v>-34.656092</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P370" t="inlineStr">
@@ -28481,7 +28481,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -28491,22 +28491,22 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D371" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E371" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G371" t="inlineStr">
@@ -28538,14 +28538,14 @@
         </is>
       </c>
       <c r="M371" t="n">
-        <v>-58.375684</v>
+        <v>-58.401374</v>
       </c>
       <c r="N371" t="n">
-        <v>-34.656092</v>
+        <v>-34.592623</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P371" t="inlineStr">
@@ -28557,7 +28557,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
@@ -28567,17 +28567,17 @@
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E372" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
@@ -28592,7 +28592,7 @@
       </c>
       <c r="H372" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I372" t="n">
@@ -28600,7 +28600,7 @@
       </c>
       <c r="J372" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K372" t="inlineStr">
@@ -28614,14 +28614,14 @@
         </is>
       </c>
       <c r="M372" t="n">
-        <v>-58.401374</v>
+        <v>-58.403444</v>
       </c>
       <c r="N372" t="n">
-        <v>-34.592623</v>
+        <v>-34.61685</v>
       </c>
       <c r="O372" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P372" t="inlineStr">
@@ -28633,7 +28633,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>-547</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
@@ -28643,22 +28643,22 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>Habana 4210</t>
         </is>
       </c>
       <c r="D373" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E373" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808733921</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G373" t="inlineStr">
@@ -28668,7 +28668,7 @@
       </c>
       <c r="H373" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar poste dañado</t>
         </is>
       </c>
       <c r="I373" t="n">
@@ -28686,30 +28686,30 @@
       </c>
       <c r="L373" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M373" t="n">
-        <v>-58.403444</v>
+        <v>-58.515873</v>
       </c>
       <c r="N373" t="n">
-        <v>-34.61685</v>
+        <v>-34.599425</v>
       </c>
       <c r="O373" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P373" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>-547</t>
+          <t>-548</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -28719,22 +28719,22 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>Habana 4210</t>
+          <t>Sucre 1533</t>
         </is>
       </c>
       <c r="D374" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E374" t="inlineStr">
         <is>
-          <t>808733921</t>
+          <t xml:space="preserve">ICD30326446 </t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>Optical Power</t>
         </is>
       </c>
       <c r="G374" t="inlineStr">
@@ -28744,7 +28744,7 @@
       </c>
       <c r="H374" t="inlineStr">
         <is>
-          <t>Cambiar poste dañado</t>
+          <t>Traspasar red a columna de TLC y Retirar columna quebrada</t>
         </is>
       </c>
       <c r="I374" t="n">
@@ -28752,7 +28752,7 @@
       </c>
       <c r="J374" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K374" t="inlineStr">
@@ -28762,18 +28762,18 @@
       </c>
       <c r="L374" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M374" t="n">
-        <v>-58.515873</v>
+        <v>-58.44649</v>
       </c>
       <c r="N374" t="n">
-        <v>-34.599425</v>
+        <v>-34.558808</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P374" t="inlineStr">
@@ -28785,17 +28785,17 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>-548</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>Sucre 1533</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D375" t="inlineStr">
@@ -28805,12 +28805,12 @@
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
         <is>
-          <t>Optical Power</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G375" t="inlineStr">
@@ -28820,7 +28820,7 @@
       </c>
       <c r="H375" t="inlineStr">
         <is>
-          <t>Traspasar red a columna de TLC y Retirar columna quebrada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I375" t="n">
@@ -28828,7 +28828,7 @@
       </c>
       <c r="J375" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K375" t="inlineStr">
@@ -28838,21 +28838,97 @@
       </c>
       <c r="L375" t="inlineStr">
         <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M375" t="n">
+        <v>-58.461024</v>
+      </c>
+      <c r="N375" t="n">
+        <v>-34.539409</v>
+      </c>
+      <c r="O375" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P375" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>-549</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>8/7/2025</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>14 de Julio 65</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>808749189</t>
+        </is>
+      </c>
+      <c r="F376" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G376" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H376" t="inlineStr">
+        <is>
+          <t>picada</t>
+        </is>
+      </c>
+      <c r="I376" t="n">
+        <v>1</v>
+      </c>
+      <c r="J376" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K376" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L376" t="inlineStr">
+        <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M375" t="n">
-        <v>-58.44649</v>
-      </c>
-      <c r="N375" t="n">
-        <v>-34.558808</v>
-      </c>
-      <c r="O375" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P375" t="inlineStr">
+      <c r="M376" t="n">
+        <v>-58.468496</v>
+      </c>
+      <c r="N376" t="n">
+        <v>-34.591282</v>
+      </c>
+      <c r="O376" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P376" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>
@@ -28869,7 +28945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30413,7 +30489,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Retirar PRFV telecentro ya traspaso nodo</t>
+          <t>Telecentro ya traspaso su nodo solo falta desmontar el prfv que quedo</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -33829,7 +33905,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -34858,7 +34934,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>-541</t>
+          <t>6578</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -34878,7 +34954,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808663880</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -35086,17 +35162,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-545</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Jeronimo Salguero 3601</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -35106,7 +35182,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808713766</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -35121,7 +35197,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Chocada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -35129,7 +35205,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -35143,10 +35219,10 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.400953</v>
+        <v>-58.401374</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.572274</v>
+        <v>-34.592623</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -35162,7 +35238,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -35172,17 +35248,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -35197,7 +35273,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -35205,7 +35281,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -35219,93 +35295,17 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.401374</v>
+        <v>-58.403444</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.592623</v>
+        <v>-34.61685</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>6572</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>8/6/2025</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>MEXICO 2639</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>808733920</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I85" t="n">
-        <v>1</v>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M85" t="n">
-        <v>-58.403444</v>
-      </c>
-      <c r="N85" t="n">
-        <v>-34.61685</v>
-      </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P85" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
@@ -42415,7 +42415,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t xml:space="preserve">ICD30326446 </t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -42479,7 +42479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -47032,6 +47032,82 @@
         </is>
       </c>
       <c r="P60" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>6579</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>8/7/2025</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>808749184</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Poste inclinado</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M61" t="n">
+        <v>-58.461024</v>
+      </c>
+      <c r="N61" t="n">
+        <v>-34.539409</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>
@@ -47377,7 +47453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P86"/>
+  <dimension ref="A1:P87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -52998,7 +53074,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-518</t>
+          <t>6585</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -53904,6 +53980,82 @@
       <c r="P86" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>-549</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>8/7/2025</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>14 de Julio 65</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>808749189</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>picada</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M87" t="n">
+        <v>-58.468496</v>
+      </c>
+      <c r="N87" t="n">
+        <v>-34.591282</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
@@ -56891,7 +57043,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-512</t>
+          <t>6580</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-15 11:46:37)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -3165,7 +3165,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>ICD30399325</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3885,10 +3885,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr"/>
-      <c r="P46" t="inlineStr"/>
+      <c r="M46" t="n">
+        <v>-58.432658</v>
+      </c>
+      <c r="N46" t="n">
+        <v>-34.576446</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -22297,10 +22309,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M289" t="inlineStr"/>
-      <c r="N289" t="inlineStr"/>
-      <c r="O289" t="inlineStr"/>
-      <c r="P289" t="inlineStr"/>
+      <c r="M289" t="n">
+        <v>-58.452583</v>
+      </c>
+      <c r="N289" t="n">
+        <v>-34.558668</v>
+      </c>
+      <c r="O289" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P289" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -29201,10 +29225,22 @@
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M380" t="inlineStr"/>
-      <c r="N380" t="inlineStr"/>
-      <c r="O380" t="inlineStr"/>
-      <c r="P380" t="inlineStr"/>
+      <c r="M380" t="n">
+        <v>-58.505375</v>
+      </c>
+      <c r="N380" t="n">
+        <v>-34.588299</v>
+      </c>
+      <c r="O380" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P380" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -29265,10 +29301,22 @@
           <t>Poste</t>
         </is>
       </c>
-      <c r="M381" t="inlineStr"/>
-      <c r="N381" t="inlineStr"/>
-      <c r="O381" t="inlineStr"/>
-      <c r="P381" t="inlineStr"/>
+      <c r="M381" t="n">
+        <v>-58.460834</v>
+      </c>
+      <c r="N381" t="n">
+        <v>-34.573753</v>
+      </c>
+      <c r="O381" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P381" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -29329,10 +29377,22 @@
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M382" t="inlineStr"/>
-      <c r="N382" t="inlineStr"/>
-      <c r="O382" t="inlineStr"/>
-      <c r="P382" t="inlineStr"/>
+      <c r="M382" t="n">
+        <v>-58.436264</v>
+      </c>
+      <c r="N382" t="n">
+        <v>-34.578942</v>
+      </c>
+      <c r="O382" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P382" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
@@ -29393,10 +29453,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M383" t="inlineStr"/>
-      <c r="N383" t="inlineStr"/>
-      <c r="O383" t="inlineStr"/>
-      <c r="P383" t="inlineStr"/>
+      <c r="M383" t="n">
+        <v>-58.414185</v>
+      </c>
+      <c r="N383" t="n">
+        <v>-34.64524</v>
+      </c>
+      <c r="O383" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P383" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -29457,10 +29529,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M384" t="inlineStr"/>
-      <c r="N384" t="inlineStr"/>
-      <c r="O384" t="inlineStr"/>
-      <c r="P384" t="inlineStr"/>
+      <c r="M384" t="n">
+        <v>-58.404946</v>
+      </c>
+      <c r="N384" t="n">
+        <v>-34.617251</v>
+      </c>
+      <c r="O384" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P384" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
@@ -29521,10 +29605,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M385" t="inlineStr"/>
-      <c r="N385" t="inlineStr"/>
-      <c r="O385" t="inlineStr"/>
-      <c r="P385" t="inlineStr"/>
+      <c r="M385" t="n">
+        <v>-58.460818</v>
+      </c>
+      <c r="N385" t="n">
+        <v>-34.618934</v>
+      </c>
+      <c r="O385" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P385" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
@@ -29585,10 +29681,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M386" t="inlineStr"/>
-      <c r="N386" t="inlineStr"/>
-      <c r="O386" t="inlineStr"/>
-      <c r="P386" t="inlineStr"/>
+      <c r="M386" t="n">
+        <v>-58.441171</v>
+      </c>
+      <c r="N386" t="n">
+        <v>-34.574547</v>
+      </c>
+      <c r="O386" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P386" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
@@ -29649,10 +29757,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M387" t="inlineStr"/>
-      <c r="N387" t="inlineStr"/>
-      <c r="O387" t="inlineStr"/>
-      <c r="P387" t="inlineStr"/>
+      <c r="M387" t="n">
+        <v>-58.435072</v>
+      </c>
+      <c r="N387" t="n">
+        <v>-34.565732</v>
+      </c>
+      <c r="O387" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P387" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
@@ -29713,10 +29833,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M388" t="inlineStr"/>
-      <c r="N388" t="inlineStr"/>
-      <c r="O388" t="inlineStr"/>
-      <c r="P388" t="inlineStr"/>
+      <c r="M388" t="n">
+        <v>-58.404058</v>
+      </c>
+      <c r="N388" t="n">
+        <v>-34.634341</v>
+      </c>
+      <c r="O388" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P388" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
@@ -29777,10 +29909,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M389" t="inlineStr"/>
-      <c r="N389" t="inlineStr"/>
-      <c r="O389" t="inlineStr"/>
-      <c r="P389" t="inlineStr"/>
+      <c r="M389" t="n">
+        <v>-58.487821</v>
+      </c>
+      <c r="N389" t="n">
+        <v>-34.554603</v>
+      </c>
+      <c r="O389" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P389" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
@@ -29843,8 +29987,16 @@
       </c>
       <c r="M390" t="inlineStr"/>
       <c r="N390" t="inlineStr"/>
-      <c r="O390" t="inlineStr"/>
-      <c r="P390" t="inlineStr"/>
+      <c r="O390" t="inlineStr">
+        <is>
+          <t>No ubicado</t>
+        </is>
+      </c>
+      <c r="P390" t="inlineStr">
+        <is>
+          <t>No clasificado, consultar con mantenimiento</t>
+        </is>
+      </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
@@ -29907,8 +30059,16 @@
       </c>
       <c r="M391" t="inlineStr"/>
       <c r="N391" t="inlineStr"/>
-      <c r="O391" t="inlineStr"/>
-      <c r="P391" t="inlineStr"/>
+      <c r="O391" t="inlineStr">
+        <is>
+          <t>No ubicado</t>
+        </is>
+      </c>
+      <c r="P391" t="inlineStr">
+        <is>
+          <t>No clasificado, consultar con mantenimiento</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -31446,7 +31606,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>ICD30399325</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -36190,10 +36350,22 @@
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M83" t="inlineStr"/>
-      <c r="N83" t="inlineStr"/>
-      <c r="O83" t="inlineStr"/>
-      <c r="P83" t="inlineStr"/>
+      <c r="M83" t="n">
+        <v>-58.505375</v>
+      </c>
+      <c r="N83" t="n">
+        <v>-34.588299</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -48444,10 +48616,22 @@
           <t>Poste</t>
         </is>
       </c>
-      <c r="M66" t="inlineStr"/>
-      <c r="N66" t="inlineStr"/>
-      <c r="O66" t="inlineStr"/>
-      <c r="P66" t="inlineStr"/>
+      <c r="M66" t="n">
+        <v>-58.460834</v>
+      </c>
+      <c r="N66" t="n">
+        <v>-34.573753</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -48508,10 +48692,22 @@
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M67" t="inlineStr"/>
-      <c r="N67" t="inlineStr"/>
-      <c r="O67" t="inlineStr"/>
-      <c r="P67" t="inlineStr"/>
+      <c r="M67" t="n">
+        <v>-58.436264</v>
+      </c>
+      <c r="N67" t="n">
+        <v>-34.578942</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -48572,10 +48768,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M68" t="inlineStr"/>
-      <c r="N68" t="inlineStr"/>
-      <c r="O68" t="inlineStr"/>
-      <c r="P68" t="inlineStr"/>
+      <c r="M68" t="n">
+        <v>-58.441171</v>
+      </c>
+      <c r="N68" t="n">
+        <v>-34.574547</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -48636,10 +48844,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M69" t="inlineStr"/>
-      <c r="N69" t="inlineStr"/>
-      <c r="O69" t="inlineStr"/>
-      <c r="P69" t="inlineStr"/>
+      <c r="M69" t="n">
+        <v>-58.435072</v>
+      </c>
+      <c r="N69" t="n">
+        <v>-34.565732</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -49358,10 +49578,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>-58.432658</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-34.576446</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -54418,10 +54650,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M72" t="inlineStr"/>
-      <c r="N72" t="inlineStr"/>
-      <c r="O72" t="inlineStr"/>
-      <c r="P72" t="inlineStr"/>
+      <c r="M72" t="n">
+        <v>-58.452583</v>
+      </c>
+      <c r="N72" t="n">
+        <v>-34.558668</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P72" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -55622,10 +55866,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M88" t="inlineStr"/>
-      <c r="N88" t="inlineStr"/>
-      <c r="O88" t="inlineStr"/>
-      <c r="P88" t="inlineStr"/>
+      <c r="M88" t="n">
+        <v>-58.414185</v>
+      </c>
+      <c r="N88" t="n">
+        <v>-34.64524</v>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P88" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -55686,10 +55942,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M89" t="inlineStr"/>
-      <c r="N89" t="inlineStr"/>
-      <c r="O89" t="inlineStr"/>
-      <c r="P89" t="inlineStr"/>
+      <c r="M89" t="n">
+        <v>-58.404946</v>
+      </c>
+      <c r="N89" t="n">
+        <v>-34.617251</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -55750,10 +56018,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M90" t="inlineStr"/>
-      <c r="N90" t="inlineStr"/>
-      <c r="O90" t="inlineStr"/>
-      <c r="P90" t="inlineStr"/>
+      <c r="M90" t="n">
+        <v>-58.460818</v>
+      </c>
+      <c r="N90" t="n">
+        <v>-34.618934</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -59631,10 +59911,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr"/>
+      <c r="M51" t="n">
+        <v>-58.404058</v>
+      </c>
+      <c r="N51" t="n">
+        <v>-34.634341</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -59695,10 +59987,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
-      <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr"/>
+      <c r="M52" t="n">
+        <v>-58.487821</v>
+      </c>
+      <c r="N52" t="n">
+        <v>-34.554603</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -59761,8 +60065,16 @@
       </c>
       <c r="M53" t="inlineStr"/>
       <c r="N53" t="inlineStr"/>
-      <c r="O53" t="inlineStr"/>
-      <c r="P53" t="inlineStr"/>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>No ubicado</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>No clasificado, consultar con mantenimiento</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -59825,8 +60137,16 @@
       </c>
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="inlineStr"/>
-      <c r="O54" t="inlineStr"/>
-      <c r="P54" t="inlineStr"/>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>No ubicado</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>No clasificado, consultar con mantenimiento</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-25 10:39:17)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -27370,7 +27370,7 @@
       </c>
       <c r="F356" t="inlineStr">
         <is>
-          <t>Optical Power</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G356" t="inlineStr">
@@ -27380,7 +27380,7 @@
       </c>
       <c r="H356" t="inlineStr">
         <is>
-          <t>Traspasar red a columna de TLC y Retirar columna quebrada</t>
+          <t>Retirar columna</t>
         </is>
       </c>
       <c r="I356" t="n">
@@ -30385,7 +30385,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P82"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35990,27 +35990,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6002</t>
+          <t>-548</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 832</t>
+          <t>Sucre 1533</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808918694</t>
+          <t xml:space="preserve">ICD30326446 </t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -36025,7 +36025,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Retirar columna</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -36033,7 +36033,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -36047,26 +36047,26 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.426947</v>
+        <v>-58.44649</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.625698</v>
+        <v>-34.558808</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>6002</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -36076,17 +36076,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>LA PLATA AV. 832</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808918694</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -36101,7 +36101,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -36123,14 +36123,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.402657</v>
+        <v>-58.426947</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.592182</v>
+        <v>-34.625698</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -36142,7 +36142,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-551</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -36152,17 +36152,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Estados Unidos 2044</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -36177,7 +36177,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -36199,14 +36199,14 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.395142</v>
+        <v>-58.402657</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.619586</v>
+        <v>-34.592182</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -36218,27 +36218,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6907</t>
+          <t>-551</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 3142</t>
+          <t>Estados Unidos 2044</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>ICD30401322</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -36253,7 +36253,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -36261,7 +36261,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -36271,50 +36271,50 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.505375</v>
+        <v>-58.395142</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.588299</v>
+        <v>-34.619586</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>6907</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>Av. Gral. Mosconi 3142</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>ICD30401322</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -36324,12 +36324,12 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -36337,40 +36337,40 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.413584</v>
+        <v>-58.505375</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.58551</v>
+        <v>-34.588299</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -36380,7 +36380,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -36390,7 +36390,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -36400,12 +36400,12 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -36418,7 +36418,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
@@ -36427,10 +36427,10 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.419711</v>
+        <v>-58.413584</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.586299</v>
+        <v>-34.58551</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -36446,7 +36446,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -36456,17 +36456,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -36481,7 +36481,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -36499,18 +36499,18 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.437583</v>
+        <v>-58.419711</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.616231</v>
+        <v>-34.586299</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -36522,74 +36522,150 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
+          <t>5625</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>8/20/2025</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>ACOYTE AV. 184</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>809065913</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Inclinada ver cambio</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>-58.437583</v>
+      </c>
+      <c r="N82" t="n">
+        <v>-34.616231</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
           <t>-560</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
+      <c r="B83" t="inlineStr">
         <is>
           <t>8/21/2025</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
+      <c r="C83" t="inlineStr">
         <is>
           <t>Pinzon 1590</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
+      <c r="D83" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr">
+      <c r="E83" t="inlineStr">
         <is>
           <t>809098712</t>
         </is>
       </c>
-      <c r="F82" t="inlineStr">
+      <c r="F83" t="inlineStr">
         <is>
           <t>PEBCOM</t>
         </is>
       </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
         <is>
           <t>Picada</t>
         </is>
       </c>
-      <c r="I82" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M82" t="n">
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M83" t="n">
         <v>-58.373506</v>
       </c>
-      <c r="N82" t="n">
+      <c r="N83" t="n">
         <v>-34.63706</v>
       </c>
-      <c r="O82" t="inlineStr">
+      <c r="O83" t="inlineStr">
         <is>
           <t>San Telmo</t>
         </is>
       </c>
-      <c r="P82" t="inlineStr">
+      <c r="P83" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
@@ -36606,7 +36682,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P96"/>
+  <dimension ref="A1:P95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -43755,27 +43831,27 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>-548</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Sucre 1533</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30326446 </t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -43790,7 +43866,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Traspasar red a columna de TLC y Retirar columna quebrada</t>
+          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
         </is>
       </c>
       <c r="I95" t="n">
@@ -43798,7 +43874,7 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
@@ -43812,93 +43888,17 @@
         </is>
       </c>
       <c r="M95" t="n">
-        <v>-58.44649</v>
+        <v>-58.355342</v>
       </c>
       <c r="N95" t="n">
-        <v>-34.558808</v>
+        <v>-34.63565</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P95" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>6917</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>8/12/2025</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>BRIN, MINISTRO 1375</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>808918700</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
-        </is>
-      </c>
-      <c r="I96" t="n">
-        <v>1</v>
-      </c>
-      <c r="J96" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M96" t="n">
-        <v>-58.355342</v>
-      </c>
-      <c r="N96" t="n">
-        <v>-34.63565</v>
-      </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P96" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-25 12:54:13)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P395"/>
+  <dimension ref="A1:P397"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24609,7 +24609,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>7023</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -24619,7 +24619,7 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>ZABALA 3573</t>
         </is>
       </c>
       <c r="D320" t="inlineStr">
@@ -24666,10 +24666,10 @@
         </is>
       </c>
       <c r="M320" t="n">
-        <v>-58.457492</v>
+        <v>-58.457522</v>
       </c>
       <c r="N320" t="n">
-        <v>-34.579336</v>
+        <v>-34.579414</v>
       </c>
       <c r="O320" t="inlineStr">
         <is>
@@ -30371,6 +30371,158 @@
       <c r="P395" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>7024</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>SAAVEDRA 869</t>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>809155616</t>
+        </is>
+      </c>
+      <c r="F396" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G396" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H396" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I396" t="n">
+        <v>1</v>
+      </c>
+      <c r="J396" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K396" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L396" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M396" t="n">
+        <v>-58.402244</v>
+      </c>
+      <c r="N396" t="n">
+        <v>-34.619401</v>
+      </c>
+      <c r="O396" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P396" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>7021</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>VERA 445</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>809155622</t>
+        </is>
+      </c>
+      <c r="F397" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G397" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H397" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I397" t="n">
+        <v>1</v>
+      </c>
+      <c r="J397" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K397" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L397" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M397" t="n">
+        <v>-58.437181</v>
+      </c>
+      <c r="N397" t="n">
+        <v>-34.5995</v>
+      </c>
+      <c r="O397" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P397" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
@@ -30385,7 +30537,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36666,6 +36818,82 @@
         </is>
       </c>
       <c r="P83" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>7024</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>SAAVEDRA 869</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>809155616</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>-58.402244</v>
+      </c>
+      <c r="N84" t="n">
+        <v>-34.619401</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
@@ -44168,7 +44396,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P74"/>
+  <dimension ref="A1:P75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -47901,7 +48129,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-525</t>
+          <t>7023</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -47911,7 +48139,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Zabala 3567</t>
+          <t>ZABALA 3573</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -47958,10 +48186,10 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.457492</v>
+        <v>-58.457522</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.579336</v>
+        <v>-34.579414</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -49795,6 +50023,82 @@
       <c r="P74" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>7021</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>VERA 445</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>809155622</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M75" t="n">
+        <v>-58.437181</v>
+      </c>
+      <c r="N75" t="n">
+        <v>-34.5995</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-25 13:59:42)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P397"/>
+  <dimension ref="A1:P399"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30521,6 +30521,158 @@
         </is>
       </c>
       <c r="P397" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>809156751</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>Av San Martín 5045</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>809156751</t>
+        </is>
+      </c>
+      <c r="F398" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G398" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H398" t="inlineStr">
+        <is>
+          <t>aplomar o cambiar poste de 11 con rienda a pique</t>
+        </is>
+      </c>
+      <c r="I398" t="n">
+        <v>0</v>
+      </c>
+      <c r="J398" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K398" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L398" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M398" t="n">
+        <v>-58.489141</v>
+      </c>
+      <c r="N398" t="n">
+        <v>-34.597221</v>
+      </c>
+      <c r="O398" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P398" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>-563</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>Av Castañares 4520</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>809157022</t>
+        </is>
+      </c>
+      <c r="F399" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G399" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H399" t="inlineStr">
+        <is>
+          <t>Cambiar pasante</t>
+        </is>
+      </c>
+      <c r="I399" t="n">
+        <v>1</v>
+      </c>
+      <c r="J399" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K399" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L399" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M399" t="n">
+        <v>-58.470249</v>
+      </c>
+      <c r="N399" t="n">
+        <v>-34.664835</v>
+      </c>
+      <c r="O399" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P399" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
@@ -50113,7 +50265,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P88"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -56790,6 +56942,82 @@
         </is>
       </c>
       <c r="P88" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>-563</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Av Castañares 4520</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>809157022</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Cambiar pasante</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>1</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>-58.470249</v>
+      </c>
+      <c r="N89" t="n">
+        <v>-34.664835</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
@@ -60843,7 +61071,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -61237,6 +61465,82 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>809156751</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Av San Martín 5045</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>809156751</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>aplomar o cambiar poste de 11 con rienda a pique</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>-58.489141</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-34.597221</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-26 06:53:53)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P399"/>
+  <dimension ref="A1:P401"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -630,11 +630,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Nodo transferido, retirar columna</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
         <v>1</v>
       </c>
@@ -30673,6 +30669,158 @@
         </is>
       </c>
       <c r="P399" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>-564</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>Quito 3666</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>809168441</t>
+        </is>
+      </c>
+      <c r="F400" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G400" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H400" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I400" t="n">
+        <v>1</v>
+      </c>
+      <c r="J400" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K400" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L400" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M400" t="n">
+        <v>-58.41791</v>
+      </c>
+      <c r="N400" t="n">
+        <v>-34.616706</v>
+      </c>
+      <c r="O400" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P400" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>-565</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>Venezuela 3888</t>
+        </is>
+      </c>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>809168446</t>
+        </is>
+      </c>
+      <c r="F401" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G401" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H401" t="inlineStr">
+        <is>
+          <t>PIcada</t>
+        </is>
+      </c>
+      <c r="I401" t="n">
+        <v>1</v>
+      </c>
+      <c r="J401" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K401" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L401" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M401" t="n">
+        <v>-58.420309</v>
+      </c>
+      <c r="N401" t="n">
+        <v>-34.61767</v>
+      </c>
+      <c r="O401" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P401" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
@@ -30887,11 +31035,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Nodo transferido, retirar columna</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
         <v>1</v>
       </c>
@@ -61071,7 +61215,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -61541,6 +61685,158 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>-564</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Quito 3666</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>809168441</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>-58.41791</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-34.616706</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>-565</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Venezuela 3888</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>809168446</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>PIcada</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>-58.420309</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-34.61767</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-26 08:54:14)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P401"/>
+  <dimension ref="A1:P402"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30823,6 +30823,82 @@
       <c r="P401" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>-566</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>Asuncion 2710</t>
+        </is>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E402" t="inlineStr">
+        <is>
+          <t>809171103</t>
+        </is>
+      </c>
+      <c r="F402" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G402" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H402" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="I402" t="n">
+        <v>0</v>
+      </c>
+      <c r="J402" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K402" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L402" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M402" t="n">
+        <v>-58.494789</v>
+      </c>
+      <c r="N402" t="n">
+        <v>-34.59082</v>
+      </c>
+      <c r="O402" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P402" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
@@ -30837,7 +30913,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37192,6 +37268,82 @@
       <c r="P84" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>-566</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Asuncion 2710</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>809171103</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
+        <v>-58.494789</v>
+      </c>
+      <c r="N85" t="n">
+        <v>-34.59082</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-26 10:33:13)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P402"/>
+  <dimension ref="A1:P403"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30897,6 +30897,82 @@
         </is>
       </c>
       <c r="P402" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>-567</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>Franco 2543</t>
+        </is>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>809184735</t>
+        </is>
+      </c>
+      <c r="F403" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G403" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H403" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="I403" t="n">
+        <v>0</v>
+      </c>
+      <c r="J403" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K403" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L403" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M403" t="n">
+        <v>-58.502565</v>
+      </c>
+      <c r="N403" t="n">
+        <v>-34.578977</v>
+      </c>
+      <c r="O403" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P403" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>
@@ -44844,7 +44920,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P75"/>
+  <dimension ref="A1:P76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50547,6 +50623,82 @@
       <c r="P75" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>-567</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Franco 2543</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>809184735</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M76" t="n">
+        <v>-58.502565</v>
+      </c>
+      <c r="N76" t="n">
+        <v>-34.578977</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-26 21:27:09)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -5421,7 +5421,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Pendiente ICD</t>
+          <t>ICD30501795</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -23485,7 +23485,7 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>ICD30501825</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -32434,7 +32434,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Pendiente ICD</t>
+          <t>ICD30501795</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -43995,7 +43995,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>ICD30501825</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-28 07:06:19)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P395"/>
+  <dimension ref="A1:P396"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29005,7 +29005,7 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>-557</t>
+          <t>7072</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
@@ -29015,7 +29015,7 @@
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>Av Castañares 4621</t>
+          <t>CASTAÑARES AV. 4611</t>
         </is>
       </c>
       <c r="D378" t="inlineStr">
@@ -29025,7 +29025,7 @@
       </c>
       <c r="E378" t="inlineStr">
         <is>
-          <t>ICD30462144</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
@@ -29035,12 +29035,12 @@
       </c>
       <c r="G378" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H378" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo telecom</t>
+          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
         </is>
       </c>
       <c r="I378" t="n">
@@ -29056,16 +29056,12 @@
           <t>Nodo Teco</t>
         </is>
       </c>
-      <c r="L378" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+      <c r="L378" t="inlineStr"/>
       <c r="M378" t="n">
-        <v>-58.470977</v>
+        <v>-58.470919</v>
       </c>
       <c r="N378" t="n">
-        <v>-34.665358</v>
+        <v>-34.665309</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>
@@ -30367,6 +30363,82 @@
       <c r="P395" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>7064</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>GAONA AV. 1189</t>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>809257408</t>
+        </is>
+      </c>
+      <c r="F396" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G396" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H396" t="inlineStr">
+        <is>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+        </is>
+      </c>
+      <c r="I396" t="n">
+        <v>1</v>
+      </c>
+      <c r="J396" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K396" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L396" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M396" t="n">
+        <v>-58.446008</v>
+      </c>
+      <c r="N396" t="n">
+        <v>-34.607602</v>
+      </c>
+      <c r="O396" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P396" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
@@ -30381,7 +30453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36658,6 +36730,82 @@
         </is>
       </c>
       <c r="P83" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>7064</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>GAONA AV. 1189</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>809257408</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>-58.446008</v>
+      </c>
+      <c r="N84" t="n">
+        <v>-34.607602</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
@@ -56030,7 +56178,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>-557</t>
+          <t>7072</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -56040,7 +56188,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Av Castañares 4621</t>
+          <t>CASTAÑARES AV. 4611</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -56050,7 +56198,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>ICD30462144</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -56060,12 +56208,12 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo telecom</t>
+          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -56081,16 +56229,12 @@
           <t>Nodo Teco</t>
         </is>
       </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+      <c r="L85" t="inlineStr"/>
       <c r="M85" t="n">
-        <v>-58.470977</v>
+        <v>-58.470919</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.665358</v>
+        <v>-34.665309</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-04 07:53:44)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P393"/>
+  <dimension ref="A1:P394"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30211,6 +30211,78 @@
       <c r="P393" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>-581</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>9/4/2025</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>Praga 1380</t>
+        </is>
+      </c>
+      <c r="D394" t="inlineStr"/>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>809432814</t>
+        </is>
+      </c>
+      <c r="F394" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G394" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H394" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I394" t="n">
+        <v>0</v>
+      </c>
+      <c r="J394" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K394" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L394" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M394" t="n">
+        <v>-58.481608</v>
+      </c>
+      <c r="N394" t="n">
+        <v>-34.587837</v>
+      </c>
+      <c r="O394" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P394" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
@@ -49797,7 +49869,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P78"/>
+  <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -55712,6 +55784,78 @@
       <c r="P78" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>-581</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>9/4/2025</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Praga 1380</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>809432814</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M79" t="n">
+        <v>-58.481608</v>
+      </c>
+      <c r="N79" t="n">
+        <v>-34.587837</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-04 08:04:11)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -13462,7 +13462,7 @@
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>INCO</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G173" t="inlineStr">
@@ -21286,7 +21286,7 @@
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>INCO</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G276" t="inlineStr">
@@ -21438,7 +21438,7 @@
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>INCO</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G278" t="inlineStr">
@@ -21666,7 +21666,7 @@
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>INCO</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G281" t="inlineStr">
@@ -22578,7 +22578,7 @@
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>INCO</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G293" t="inlineStr">
@@ -49869,7 +49869,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P79"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -52986,27 +52986,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -53043,14 +53043,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.387847</v>
+        <v>-58.372751</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.587043</v>
+        <v>-34.631917</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -53062,27 +53062,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -53097,7 +53097,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -53119,26 +53119,26 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.451835</v>
+        <v>-58.387847</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.562646</v>
+        <v>-34.587043</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -53148,17 +53148,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -53173,7 +53173,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -53181,7 +53181,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -53191,18 +53191,18 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.470837</v>
+        <v>-58.451835</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.545751</v>
+        <v>-34.562646</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -53214,7 +53214,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -53224,7 +53224,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -53234,7 +53234,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -53249,7 +53249,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -53262,19 +53262,19 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.472267</v>
+        <v>-58.470837</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.551163</v>
+        <v>-34.545751</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -53290,27 +53290,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -53325,7 +53325,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -53333,12 +53333,12 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -53347,10 +53347,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.464144</v>
+        <v>-58.472267</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.541832</v>
+        <v>-34.551163</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -53366,7 +53366,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -53376,17 +53376,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -53401,7 +53401,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -53423,26 +53423,26 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.434761</v>
+        <v>-58.464144</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.598381</v>
+        <v>-34.541832</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -53452,17 +53452,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -53477,7 +53477,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -53495,30 +53495,30 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.464177</v>
+        <v>-58.434761</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.558239</v>
+        <v>-34.598381</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -53528,17 +53528,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -53553,7 +53553,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -53571,50 +53571,50 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.412302</v>
+        <v>-58.464177</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.59301</v>
+        <v>-34.558239</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -53629,11 +53629,11 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -53651,46 +53651,46 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.485056</v>
+        <v>-58.412302</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.555059</v>
+        <v>-34.59301</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/22/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Cucha Cucha 2918</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -53705,15 +53705,15 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -53727,14 +53727,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.469783</v>
+        <v>-58.485056</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.599214</v>
+        <v>-34.555059</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -53746,27 +53746,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>807044233</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/22/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Martin Grandoli 5761</t>
+          <t>Cucha Cucha 2918</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30261461 </t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -53781,7 +53781,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -53789,7 +53789,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -53799,50 +53799,50 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.487144</v>
+        <v>-58.469783</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.669078</v>
+        <v>-34.599214</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Martin Grandoli 5761</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t xml:space="preserve">ICD30261461 </t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -53855,13 +53855,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr"/>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
+        </is>
+      </c>
       <c r="I53" t="n">
         <v>1</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -53871,18 +53875,18 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.405761</v>
+        <v>-58.487144</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.582476</v>
+        <v>-34.669078</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -53894,17 +53898,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -53914,7 +53918,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -53927,11 +53931,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H54" t="inlineStr"/>
       <c r="I54" t="n">
         <v>1</v>
       </c>
@@ -53951,14 +53951,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.432241</v>
+        <v>-58.405761</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.56642</v>
+        <v>-34.582476</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -53970,7 +53970,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -53980,7 +53980,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -53990,7 +53990,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -54005,7 +54005,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -54027,10 +54027,10 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.417348</v>
+        <v>-58.432241</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.595467</v>
+        <v>-34.56642</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -54046,27 +54046,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -54081,7 +54081,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -54099,18 +54099,18 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.472311</v>
+        <v>-58.417348</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.654867</v>
+        <v>-34.595467</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -54122,7 +54122,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -54132,17 +54132,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -54157,7 +54157,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -54175,50 +54175,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.484729</v>
+        <v>-58.472311</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.574614</v>
+        <v>-34.654867</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6409</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 5656</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807965768</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -54233,7 +54233,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Faltan cargar las fotos del cierre</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -54251,50 +54251,50 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.479921</v>
+        <v>-58.484729</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.673021</v>
+        <v>-34.574614</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6409</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>CASTAÑARES AV. 5656</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>807965768</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -54309,7 +54309,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Faltan cargar las fotos del cierre</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -54317,7 +54317,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -54327,40 +54327,40 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.510247</v>
+        <v>-58.479921</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.645038</v>
+        <v>-34.673021</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6585</t>
+          <t>6580</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t>Ciudad de la Paz 3742</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -54370,7 +54370,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>808240230</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -54385,7 +54385,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -54407,10 +54407,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.483145</v>
+        <v>-58.470347</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.557043</v>
+        <v>-34.547965</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -54426,27 +54426,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6486</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Laferrere 6572</t>
+          <t>BILBAO, FRANCISCO 2442</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808243829</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -54461,7 +54461,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -54483,46 +54483,46 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.496608</v>
+        <v>-58.460522</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.666371</v>
+        <v>-34.635514</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -54537,7 +54537,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -54555,50 +54555,50 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.422229</v>
+        <v>-58.510247</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.573148</v>
+        <v>-34.645038</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6695</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>OLAZABAL AV. 4417</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808373646</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -54613,7 +54613,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -54621,7 +54621,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -54631,40 +54631,40 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.494864</v>
+        <v>-58.478941</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.678826</v>
+        <v>-34.57242</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>6585</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -54674,7 +54674,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -54689,7 +54689,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -54711,14 +54711,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.473089</v>
+        <v>-58.483145</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.625478</v>
+        <v>-34.557043</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -54730,27 +54730,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>Laferrere 6572</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -54765,7 +54765,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -54787,36 +54787,36 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.468841</v>
+        <v>-58.496608</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.686635</v>
+        <v>-34.666371</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6478</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>JUJUY AV. 1647</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -54826,7 +54826,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808509387</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -54841,7 +54841,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -54849,7 +54849,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -54863,10 +54863,10 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.375684</v>
+        <v>-58.401083</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.656092</v>
+        <v>-34.629397</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -54882,27 +54882,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6960</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 1940</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808972988</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -54917,7 +54917,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -54925,7 +54925,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -54939,14 +54939,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.460818</v>
+        <v>-58.422229</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.618934</v>
+        <v>-34.573148</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -54958,27 +54958,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/18/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 6740</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809006419</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -54993,7 +54993,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -55001,7 +55001,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -55011,14 +55011,14 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.460441</v>
+        <v>-58.494864</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.628243</v>
+        <v>-34.678826</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -55034,27 +55034,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7072</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 4611</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>ICD30519785</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -55064,12 +55064,12 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -55082,51 +55082,55 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L69" t="inlineStr"/>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M69" t="n">
-        <v>-58.470919</v>
+        <v>-58.473089</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.665309</v>
+        <v>-34.625478</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7060</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>PINZON 1578</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809195671</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -55163,14 +55167,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.373428</v>
+        <v>-58.468841</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.63705</v>
+        <v>-34.686635</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -55182,27 +55186,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-568</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Ameghino 523</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809208239</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -55217,7 +55221,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Picada con pelgro de caida</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -55225,7 +55229,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -55239,46 +55243,46 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.488424</v>
+        <v>-58.375684</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.642002</v>
+        <v>-34.656092</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>6960</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>VALLESE, FELIPE 1940</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>808972988</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -55293,7 +55297,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -55311,18 +55315,18 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.37456</v>
+        <v>-58.460818</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.649779</v>
+        <v>-34.618934</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -55334,27 +55338,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7089</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 637</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809270751</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -55369,7 +55373,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -55377,7 +55381,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -55391,14 +55395,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.37805</v>
+        <v>-58.460441</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.649722</v>
+        <v>-34.628243</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -55410,27 +55414,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>7072</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 625</t>
+          <t>CASTAÑARES AV. 4611</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809270753</t>
+          <t>ICD30519785</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -55440,12 +55444,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -55458,23 +55462,19 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L74" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr"/>
       <c r="M74" t="n">
-        <v>-58.378104</v>
+        <v>-58.470919</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.649578</v>
+        <v>-34.665309</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -55486,17 +55486,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7091</t>
+          <t>7060</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>SUAREZ AV. 1966</t>
+          <t>PINZON 1578</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -55506,7 +55506,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809279022</t>
+          <t>809195671</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -55521,7 +55521,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -55543,10 +55543,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.377974</v>
+        <v>-58.373428</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.641024</v>
+        <v>-34.63705</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -55562,27 +55562,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7096</t>
+          <t>-568</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
+          <t>Ameghino 523</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809279069</t>
+          <t>809208239</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -55597,7 +55597,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada con pelgro de caida</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -55619,46 +55619,46 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.435511</v>
+        <v>-58.488424</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.644702</v>
+        <v>-34.642002</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7106</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>MARTI, JOSE 627</t>
+          <t>HERRERA 1998</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809371835</t>
+          <t>809268244</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -55673,7 +55673,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Poste quebrado cambiar por prfv es un poste viejo ExCV</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -55691,18 +55691,18 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.469159</v>
+        <v>-58.37456</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.638898</v>
+        <v>-34.649779</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -55714,27 +55714,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>4088</t>
+          <t>7089</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>GOMEZ, VALENTIN 3648</t>
+          <t>SAN ANTONIO 637</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809406164</t>
+          <t>809270751</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -55749,7 +55749,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -55771,14 +55771,14 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.416416</v>
+        <v>-58.37805</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.604812</v>
+        <v>-34.649722</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -55790,70 +55790,450 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
+          <t>7090</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>SAN ANTONIO 625</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>809270753</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>1</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M79" t="n">
+        <v>-58.378104</v>
+      </c>
+      <c r="N79" t="n">
+        <v>-34.649578</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>7091</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>SUAREZ AV. 1966</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>809279022</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>1</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
+        <v>-58.377974</v>
+      </c>
+      <c r="N80" t="n">
+        <v>-34.641024</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>7096</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>VEDIA, AGUSTIN DE 2185</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>809279069</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>-58.435511</v>
+      </c>
+      <c r="N81" t="n">
+        <v>-34.644702</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>7106</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>9/1/2025</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>MARTI, JOSE 627</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>809371835</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Poste quebrado cambiar por prfv es un poste viejo ExCV</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>-58.469159</v>
+      </c>
+      <c r="N82" t="n">
+        <v>-34.638898</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>4088</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>9/2/2025</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>GOMEZ, VALENTIN 3648</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>809406164</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M83" t="n">
+        <v>-58.416416</v>
+      </c>
+      <c r="N83" t="n">
+        <v>-34.604812</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
           <t>-581</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="B84" t="inlineStr">
         <is>
           <t>9/4/2025</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
+      <c r="C84" t="inlineStr">
         <is>
           <t>Praga 1380</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr">
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="inlineStr">
         <is>
           <t>809432814</t>
         </is>
       </c>
-      <c r="F79" t="inlineStr">
+      <c r="F84" t="inlineStr">
         <is>
           <t>AYKO</t>
         </is>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
         <is>
           <t>Cambiar</t>
         </is>
       </c>
-      <c r="I79" t="n">
+      <c r="I84" t="n">
         <v>0</v>
       </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L79" t="inlineStr">
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M79" t="n">
+      <c r="M84" t="n">
         <v>-58.481608</v>
       </c>
-      <c r="N79" t="n">
+      <c r="N84" t="n">
         <v>-34.587837</v>
       </c>
-      <c r="O79" t="inlineStr">
+      <c r="O84" t="inlineStr">
         <is>
           <t>Paternal</t>
         </is>
       </c>
-      <c r="P79" t="inlineStr">
+      <c r="P84" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>
@@ -55870,7 +56250,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -58083,27 +58463,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>Soldado de la Independencia 1298</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>805707245</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -58118,7 +58498,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada - Con fuente teco</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -58131,7 +58511,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -58140,36 +58520,36 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.372751</v>
+        <v>-58.440507</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.631917</v>
+        <v>-34.564016</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Soldado de la Independencia 1298</t>
+          <t>Luis Maria Campos 1336</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -58179,7 +58559,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805707245</t>
+          <t>805722772</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -58194,7 +58574,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada - Con fuente teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -58207,7 +58587,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -58216,10 +58596,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.440507</v>
+        <v>-58.44191</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.564016</v>
+        <v>-34.564245</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -58235,27 +58615,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 1336</t>
+          <t>Del Barco Centenera 894</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805722772</t>
+          <t>807044216</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -58270,7 +58650,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -58288,50 +58668,50 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.44191</v>
+        <v>-58.438744</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.564245</v>
+        <v>-34.629929</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>-507</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Del Barco Centenera 894</t>
+          <t>Tamborini 3291</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>807044216</t>
+          <t>808194229</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -58346,7 +58726,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -58364,30 +58744,30 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.438744</v>
+        <v>-58.473937</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.629929</v>
+        <v>-34.557355</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-508</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -58397,7 +58777,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Tamborini 3291</t>
+          <t>Moldes 2463</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -58407,7 +58787,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>808194229</t>
+          <t>808194234</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -58435,7 +58815,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -58444,10 +58824,10 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.473937</v>
+        <v>-58.462281</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.557355</v>
+        <v>-34.560321</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -58463,7 +58843,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-508</t>
+          <t>-509</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -58473,17 +58853,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Moldes 2463</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808194234</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -58511,7 +58891,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -58520,26 +58900,26 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.462281</v>
+        <v>-58.403422</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.560321</v>
+        <v>-34.609195</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-509</t>
+          <t>-510</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -58549,7 +58929,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Larrea 590</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -58559,7 +58939,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>808194254</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -58587,7 +58967,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -58596,10 +58976,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.403422</v>
+        <v>-58.402353</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.609195</v>
+        <v>-34.602205</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -58615,27 +58995,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-510</t>
+          <t>-523</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/20/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Larrea 590</t>
+          <t>Luis Maria Campos 585</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>808194254</t>
+          <t>808460898</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -58663,7 +59043,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -58672,14 +59052,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.402353</v>
+        <v>-58.434668</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.602205</v>
+        <v>-34.571258</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -58691,27 +59071,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6580</t>
+          <t>-524</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 3742</t>
+          <t>Luis Maria Campos 509</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808240230</t>
+          <t>808460897</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -58748,36 +59128,36 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.470347</v>
+        <v>-58.434194</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.547965</v>
+        <v>-34.571754</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6486</t>
+          <t>-539</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2442</t>
+          <t>Tejedor 1097</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -58787,7 +59167,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808243829</t>
+          <t>808615951</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -58820,14 +59200,14 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.460522</v>
+        <v>-58.440748</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.635514</v>
+        <v>-34.63245</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -58843,27 +59223,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6695</t>
+          <t>-540</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>OLAZABAL AV. 4417</t>
+          <t>Tejedor 1071</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808373646</t>
+          <t>808615948</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -58900,46 +59280,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.478941</v>
+        <v>-58.44037</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.57242</v>
+        <v>-34.632249</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-523</t>
+          <t>-542</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7/20/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 585</t>
+          <t>Cramer 2141</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808460898</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -58954,7 +59334,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -58976,46 +59356,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.434668</v>
+        <v>-58.461582</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.571258</v>
+        <v>-34.564296</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-524</t>
+          <t>-546</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Luis Maria Campos 509</t>
+          <t>Albarellos 3031</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808460897</t>
+          <t>808720857</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -59052,36 +59432,36 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.434194</v>
+        <v>-58.511732</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.571754</v>
+        <v>-34.578688</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6478</t>
+          <t>-552</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>JUJUY AV. 1647</t>
+          <t>Catulo Castillo 2890</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -59091,7 +59471,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808509387</t>
+          <t>808973183</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -59128,10 +59508,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.401083</v>
+        <v>-58.404058</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.629397</v>
+        <v>-34.634341</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -59147,27 +59527,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-539</t>
+          <t>-553</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Tejedor 1097</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808615951</t>
+          <t>808973192</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -59182,7 +59562,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -59200,50 +59580,50 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.440748</v>
+        <v>-58.487821</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.63245</v>
+        <v>-34.554603</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-540</t>
+          <t>-554</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Tejedor 1071</t>
+          <t>Lima Oeste 1697</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808615948</t>
+          <t>808973197</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -59258,7 +59638,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -59266,7 +59646,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -59276,50 +59656,46 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M45" t="n">
-        <v>-58.44037</v>
-      </c>
-      <c r="N45" t="n">
-        <v>-34.632249</v>
-      </c>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-542</t>
+          <t>-555</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Cramer 2141</t>
+          <t>Lima Oeste 1649</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>808973201</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -59334,7 +59710,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -59355,390 +59731,14 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M46" t="n">
-        <v>-58.461582</v>
-      </c>
-      <c r="N46" t="n">
-        <v>-34.564296</v>
-      </c>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>-546</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>8/5/2025</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Albarellos 3031</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>808720857</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I47" t="n">
-        <v>1</v>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M47" t="n">
-        <v>-58.511732</v>
-      </c>
-      <c r="N47" t="n">
-        <v>-34.578688</v>
-      </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>-552</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Catulo Castillo 2890</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>808973183</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I48" t="n">
-        <v>1</v>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M48" t="n">
-        <v>-58.404058</v>
-      </c>
-      <c r="N48" t="n">
-        <v>-34.634341</v>
-      </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>-553</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Holmberg 4002</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>808973192</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Edificio en construcción solicitan correr columna 114 por entrada de garaje 5mts aprox Hablar con Sr Galvan encargado de la Obra</t>
-        </is>
-      </c>
-      <c r="I49" t="n">
-        <v>1</v>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M49" t="n">
-        <v>-58.487821</v>
-      </c>
-      <c r="N49" t="n">
-        <v>-34.554603</v>
-      </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>-554</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Lima Oeste 1697</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>808973197</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
-      <c r="I50" t="n">
-        <v>1</v>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr"/>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>No ubicado</t>
-        </is>
-      </c>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t>No clasificado, consultar con mantenimiento</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>-555</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Lima Oeste 1649</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>808973201</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>INCO</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I51" t="n">
-        <v>1</v>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr"/>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>No ubicado</t>
-        </is>
-      </c>
-      <c r="P51" t="inlineStr">
         <is>
           <t>No clasificado, consultar con mantenimiento</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-04 18:55:40)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -24934,7 +24934,7 @@
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G324" t="inlineStr">
@@ -30297,7 +30297,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P92"/>
+  <dimension ref="A1:P91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35746,7 +35746,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6002</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -35756,17 +35756,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 832</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808918694</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -35781,7 +35781,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -35803,14 +35803,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.426947</v>
+        <v>-58.402657</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.625698</v>
+        <v>-34.592182</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -35822,7 +35822,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>7039</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -35832,17 +35832,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>ESTADOS UNIDOS 2044</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -35857,7 +35857,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -35879,14 +35879,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.402657</v>
+        <v>-58.395142</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.592182</v>
+        <v>-34.619586</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -35898,27 +35898,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7039</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>ESTADOS UNIDOS 2044</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -35928,12 +35928,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -35946,7 +35946,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
@@ -35955,14 +35955,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.395142</v>
+        <v>-58.413584</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.619586</v>
+        <v>-34.58551</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -35974,7 +35974,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -35984,7 +35984,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -35994,7 +35994,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -36004,12 +36004,12 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -36022,7 +36022,7 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
@@ -36031,10 +36031,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.413584</v>
+        <v>-58.419711</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.58551</v>
+        <v>-34.586299</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -36050,7 +36050,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>5625</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -36060,17 +36060,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>ACOYTE AV. 184</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>809065913</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -36085,7 +36085,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada ver cambio</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -36103,18 +36103,18 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.419711</v>
+        <v>-58.437583</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.586299</v>
+        <v>-34.616231</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -36126,27 +36126,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>-560</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>Pinzon 1590</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809098712</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -36161,7 +36161,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -36179,18 +36179,18 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.437583</v>
+        <v>-58.373506</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.616231</v>
+        <v>-34.63706</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -36202,27 +36202,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-560</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Pinzon 1590</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809098712</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -36237,7 +36237,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada mismo caso que 7083</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -36259,10 +36259,10 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.373506</v>
+        <v>-58.402244</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.63706</v>
+        <v>-34.619401</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -36278,17 +36278,17 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -36298,7 +36298,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -36313,7 +36313,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada mismo caso que 7083</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -36335,14 +36335,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.402244</v>
+        <v>-58.393882</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.619401</v>
+        <v>-34.604721</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -36354,7 +36354,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -36364,7 +36364,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -36374,7 +36374,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -36411,14 +36411,14 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.393882</v>
+        <v>-58.394543</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.604721</v>
+        <v>-34.620732</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -36430,7 +36430,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -36440,17 +36440,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -36483,18 +36483,18 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.394543</v>
+        <v>-58.427206</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.620732</v>
+        <v>-34.602914</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -36506,7 +36506,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7050</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -36516,17 +36516,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>PRINGLES 788</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>809195664</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -36541,7 +36541,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -36554,7 +36554,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -36563,14 +36563,14 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.427206</v>
+        <v>-58.435017</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.602914</v>
+        <v>-34.622044</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -36582,17 +36582,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>7064</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>GAONA AV. 1189</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -36602,7 +36602,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809257408</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -36617,7 +36617,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -36630,7 +36630,7 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L84" t="inlineStr">
@@ -36639,14 +36639,14 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.435017</v>
+        <v>-58.446008</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.622044</v>
+        <v>-34.607602</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -36658,7 +36658,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7064</t>
+          <t>7097</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -36668,17 +36668,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>GAONA AV. 1189</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>809257408</t>
+          <t>809279093</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -36693,7 +36693,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -36715,14 +36715,14 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.446008</v>
+        <v>-58.458659</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.607602</v>
+        <v>-34.630464</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -36734,27 +36734,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>7097</t>
+          <t>4698</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
+          <t>REPETTO, NICOLAS, DR. 93</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>809279093</t>
+          <t>ICD30593982</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -36764,12 +36764,12 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -36782,7 +36782,7 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L86" t="inlineStr">
@@ -36791,10 +36791,10 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.458659</v>
+        <v>-58.443232</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.630464</v>
+        <v>-34.620007</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -36810,17 +36810,17 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>4698</t>
+          <t>7102</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/30/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
+          <t>AMBERES 995</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -36830,7 +36830,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>ICD30593982</t>
+          <t>809309598</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -36840,12 +36840,12 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -36858,19 +36858,19 @@
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.443232</v>
+        <v>-58.453382</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.620007</v>
+        <v>-34.612707</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
@@ -36886,27 +36886,27 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>7102</t>
+          <t>7112</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>8/30/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>AMBERES 995</t>
+          <t>OLLEROS 2488</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>809309598</t>
+          <t>809371829</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -36921,7 +36921,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -36939,18 +36939,18 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.453382</v>
+        <v>-58.444214</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.612707</v>
+        <v>-34.571197</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
@@ -36962,27 +36962,27 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>7112</t>
+          <t>7120</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>OLLEROS 2488</t>
+          <t>BLANCO ENCALADA 4210</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>809371829</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -36997,7 +36997,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Colocar R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -37010,55 +37010,55 @@
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.444214</v>
+        <v>-58.477593</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.571197</v>
+        <v>-34.570321</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>7120</t>
+          <t>7136</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/3/2025</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>BLANCO ENCALADA 4210</t>
+          <t>FERRARI 455</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809427020</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -37073,7 +37073,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir traspaso de fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I90" t="n">
@@ -37086,23 +37086,23 @@
       </c>
       <c r="K90" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M90" t="n">
-        <v>-58.477593</v>
+        <v>-58.441587</v>
       </c>
       <c r="N90" t="n">
-        <v>-34.570321</v>
+        <v>-34.60547</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
@@ -37114,7 +37114,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>7136</t>
+          <t>7150</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -37124,17 +37124,17 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>FERRARI 455</t>
+          <t>Bartolomé Mitre 3070</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>809427020</t>
+          <t>809427021</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -37149,7 +37149,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I91" t="n">
@@ -37167,97 +37167,21 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M91" t="n">
-        <v>-58.441587</v>
+        <v>-58.410025</v>
       </c>
       <c r="N91" t="n">
-        <v>-34.60547</v>
+        <v>-34.609184</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P91" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>7150</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>9/3/2025</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>Bartolomé Mitre 3070</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>809427021</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J92" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L92" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M92" t="n">
-        <v>-58.410025</v>
-      </c>
-      <c r="N92" t="n">
-        <v>-34.609184</v>
-      </c>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P92" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
@@ -44076,7 +44000,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P76"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -48189,7 +48113,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6910</t>
+          <t>6002</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -48199,17 +48123,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>RIVAS, GRAL. 2345</t>
+          <t>LA PLATA AV. 832</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808918698</t>
+          <t>808918694</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -48224,7 +48148,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -48246,26 +48170,26 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.482497</v>
+        <v>-58.426947</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.598714</v>
+        <v>-34.625698</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6928</t>
+          <t>6910</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -48275,17 +48199,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3101</t>
+          <t>RIVAS, GRAL. 2345</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808918710</t>
+          <t>808918698</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -48300,7 +48224,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -48322,10 +48246,10 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.512623</v>
+        <v>-58.482497</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.579137</v>
+        <v>-34.598714</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -48341,7 +48265,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-550</t>
+          <t>6928</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -48351,17 +48275,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Fitz roy 267</t>
+          <t>ALBARELLOS AV. 3101</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808918720</t>
+          <t>808918710</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -48376,7 +48300,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Aplomar columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -48398,10 +48322,10 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.451378</v>
+        <v>-58.512623</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.596195</v>
+        <v>-34.579137</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -48417,27 +48341,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6943</t>
+          <t>-550</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SUPERI 1459</t>
+          <t>Fitz roy 267</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808972965</t>
+          <t>808918720</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -48452,7 +48376,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Poste con base quebrada ver si es posible desmonte</t>
+          <t>Aplomar columna</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -48460,7 +48384,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -48470,18 +48394,18 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.460834</v>
+        <v>-58.451378</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.573753</v>
+        <v>-34.596195</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -48493,7 +48417,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6969</t>
+          <t>6943</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -48503,17 +48427,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 295</t>
+          <t>SUPERI 1459</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808972995</t>
+          <t>808972965</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -48528,7 +48452,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Poste con base quebrada ver si es posible desmonte</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -48536,7 +48460,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -48546,30 +48470,30 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.441171</v>
+        <v>-58.460834</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.574547</v>
+        <v>-34.573753</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6971</t>
+          <t>6969</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -48579,7 +48503,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MAURE 1594</t>
+          <t>CIUDAD DE LA PAZ 295</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -48589,7 +48513,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808973001</t>
+          <t>808972995</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -48604,7 +48528,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -48626,10 +48550,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.435072</v>
+        <v>-58.441171</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.565732</v>
+        <v>-34.574547</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -48645,17 +48569,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7000</t>
+          <t>6971</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
+          <t>MAURE 1594</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -48665,7 +48589,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>809065867</t>
+          <t>808973001</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -48680,7 +48604,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Ver de traspasar a telecentro y  desmontar ver con inspector</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -48702,10 +48626,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.420109</v>
+        <v>-58.435072</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.58764</v>
+        <v>-34.565732</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -48721,7 +48645,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7003</t>
+          <t>7000</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -48731,17 +48655,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>MELIAN AV. 2576</t>
+          <t>SCALABRINI ORTIZ, RAUL AV. 2106</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>809065874</t>
+          <t>809065867</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -48778,46 +48702,46 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.471943</v>
+        <v>-58.420109</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.564948</v>
+        <v>-34.58764</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-559</t>
+          <t>7003</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Av. Del Libertador 6736</t>
+          <t>MELIAN AV. 2576</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>809098713</t>
+          <t>809065874</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -48854,14 +48778,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.453398</v>
+        <v>-58.471943</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.550238</v>
+        <v>-34.564948</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -48873,17 +48797,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>5503</t>
+          <t>-559</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/22/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>CRAMER AV. 1771</t>
+          <t>Av. Del Libertador 6736</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -48893,7 +48817,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>809102564</t>
+          <t>809098713</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -48908,7 +48832,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -48930,14 +48854,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.458506</v>
+        <v>-58.453398</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.56783</v>
+        <v>-34.550238</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -48949,27 +48873,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>5503</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/22/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>CRAMER AV. 1771</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>809102564</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -48984,7 +48908,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -49006,10 +48930,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.472869</v>
+        <v>-58.458506</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.562</v>
+        <v>-34.56783</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -49025,7 +48949,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7080</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -49035,17 +48959,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 2196</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809125906</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -49082,14 +49006,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.459402</v>
+        <v>-58.472869</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.555262</v>
+        <v>-34.562</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -49101,7 +49025,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7021</t>
+          <t>7080</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -49111,17 +49035,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>VERA 445</t>
+          <t>UGARTE, MANUEL 2196</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809155622</t>
+          <t>809125906</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -49136,7 +49060,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Correrla para sacarla del cantero</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -49158,36 +49082,36 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.437181</v>
+        <v>-58.459402</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.5995</v>
+        <v>-34.555262</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6465</t>
+          <t>7021</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>AGUIRRE 368</t>
+          <t>VERA 445</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -49197,7 +49121,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809268249</t>
+          <t>809155622</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -49212,7 +49136,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Correrla para sacarla del cantero</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -49234,10 +49158,10 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.434651</v>
+        <v>-58.437181</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.598814</v>
+        <v>-34.5995</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -49253,7 +49177,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7095</t>
+          <t>6465</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -49263,7 +49187,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>SAN MARTIN AV. 4515</t>
+          <t>AGUIRRE 368</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -49273,7 +49197,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809268240</t>
+          <t>809268249</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -49288,7 +49212,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Columna chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -49306,30 +49230,30 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.483415</v>
+        <v>-58.434651</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.597663</v>
+        <v>-34.598814</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>-575</t>
+          <t>7095</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -49339,17 +49263,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Amenabar 3064</t>
+          <t>SAN MARTIN AV. 4515</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809281299</t>
+          <t>809268240</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -49364,7 +49288,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna chocada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -49382,18 +49306,18 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.465984</v>
+        <v>-58.483415</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.554869</v>
+        <v>-34.597663</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -49405,27 +49329,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-576</t>
+          <t>-575</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Av. Boyacá 2030</t>
+          <t>Amenabar 3064</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809309606</t>
+          <t>809281299</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -49462,14 +49386,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.471173</v>
+        <v>-58.465984</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.60704</v>
+        <v>-34.554869</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -49481,27 +49405,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7111</t>
+          <t>-576</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>VILELA 3699</t>
+          <t>Av. Boyacá 2030</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809371823</t>
+          <t>809309606</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -49516,7 +49440,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -49534,18 +49458,18 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.482817</v>
+        <v>-58.471173</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.550845</v>
+        <v>-34.60704</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -49557,17 +49481,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7118</t>
+          <t>7111</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>CUBAS, JOSE 2211</t>
+          <t>VILELA 3699</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -49577,7 +49501,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809406168</t>
+          <t>809371823</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -49592,7 +49516,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -49610,18 +49534,18 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.492448</v>
+        <v>-58.482817</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.58372</v>
+        <v>-34.550845</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -49633,7 +49557,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>-577</t>
+          <t>7118</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -49643,17 +49567,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Manuel Ugarte 2318</t>
+          <t>CUBAS, JOSE 2211</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809406177</t>
+          <t>809406168</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -49690,14 +49614,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.460635</v>
+        <v>-58.492448</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.555932</v>
+        <v>-34.58372</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -49709,7 +49633,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-578</t>
+          <t>-577</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -49719,7 +49643,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Pedro I Rivera 2536</t>
+          <t>Manuel Ugarte 2318</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -49729,7 +49653,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809406189</t>
+          <t>809406177</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -49766,10 +49690,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.462327</v>
+        <v>-58.460635</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.557565</v>
+        <v>-34.555932</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -49785,74 +49709,150 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
+          <t>-578</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>9/2/2025</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Pedro I Rivera 2536</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>809406189</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M76" t="n">
+        <v>-58.462327</v>
+      </c>
+      <c r="N76" t="n">
+        <v>-34.557565</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
           <t>-579</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
+      <c r="B77" t="inlineStr">
         <is>
           <t>9/2/2025</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="C77" t="inlineStr">
         <is>
           <t>Pedro Rivera 2546</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
+      <c r="D77" t="inlineStr">
         <is>
           <t>13</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr">
+      <c r="E77" t="inlineStr">
         <is>
           <t>ICD30612785</t>
         </is>
       </c>
-      <c r="F76" t="inlineStr">
+      <c r="F77" t="inlineStr">
         <is>
           <t>NEW</t>
         </is>
       </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
         <is>
           <t>Colocar R200 para pedir traspaso de equipos</t>
         </is>
       </c>
-      <c r="I76" t="n">
-        <v>1</v>
-      </c>
-      <c r="J76" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K76" t="inlineStr">
+      <c r="I77" t="n">
+        <v>1</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
         <is>
           <t>Nodo Teco</t>
         </is>
       </c>
-      <c r="L76" t="inlineStr">
+      <c r="L77" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M76" t="n">
+      <c r="M77" t="n">
         <v>-58.462479</v>
       </c>
-      <c r="N76" t="n">
+      <c r="N77" t="n">
         <v>-34.55765</v>
       </c>
-      <c r="O76" t="inlineStr">
+      <c r="O77" t="inlineStr">
         <is>
           <t>Saavedra</t>
         </is>
       </c>
-      <c r="P76" t="inlineStr">
+      <c r="P77" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-05 06:59:38)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P389"/>
+  <dimension ref="A1:P390"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29901,6 +29901,82 @@
         </is>
       </c>
       <c r="P389" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>-582</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>9/4/2025</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>Vilela 4019</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>809454353</t>
+        </is>
+      </c>
+      <c r="F390" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G390" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H390" t="inlineStr">
+        <is>
+          <t>Poste telefonico propio quebrado en base</t>
+        </is>
+      </c>
+      <c r="I390" t="n">
+        <v>1</v>
+      </c>
+      <c r="J390" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K390" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L390" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M390" t="n">
+        <v>-58.485872</v>
+      </c>
+      <c r="N390" t="n">
+        <v>-34.552645</v>
+      </c>
+      <c r="O390" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P390" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>
@@ -43316,7 +43392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P79"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -49321,6 +49397,82 @@
         </is>
       </c>
       <c r="P79" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>-582</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>9/4/2025</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Vilela 4019</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>809454353</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Poste telefonico propio quebrado en base</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>1</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
+        <v>-58.485872</v>
+      </c>
+      <c r="N80" t="n">
+        <v>-34.552645</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-08 10:59:39)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P387"/>
+  <dimension ref="A1:P389"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29751,6 +29751,158 @@
       <c r="P387" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>-583</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>9/8/2025</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>Av Eva Perón 1145</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>809504290</t>
+        </is>
+      </c>
+      <c r="F388" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G388" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H388" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I388" t="n">
+        <v>1</v>
+      </c>
+      <c r="J388" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K388" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L388" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M388" t="n">
+        <v>-58.441547</v>
+      </c>
+      <c r="N388" t="n">
+        <v>-34.630481</v>
+      </c>
+      <c r="O388" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P388" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>-584</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>9/8/2025</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>General Gregorio Aráoz de Lamadrid 865</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>809504300</t>
+        </is>
+      </c>
+      <c r="F389" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G389" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H389" t="inlineStr">
+        <is>
+          <t>Columna colgando</t>
+        </is>
+      </c>
+      <c r="I389" t="n">
+        <v>1</v>
+      </c>
+      <c r="J389" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K389" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L389" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M389" t="n">
+        <v>-58.364566</v>
+      </c>
+      <c r="N389" t="n">
+        <v>-34.639404</v>
+      </c>
+      <c r="O389" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P389" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
@@ -49033,7 +49185,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:P85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -55324,6 +55476,158 @@
       <c r="P83" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>-583</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>9/8/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Av Eva Perón 1145</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>809504290</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>-58.441547</v>
+      </c>
+      <c r="N84" t="n">
+        <v>-34.630481</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>-584</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>9/8/2025</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>General Gregorio Aráoz de Lamadrid 865</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>809504300</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Columna colgando</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
+        <v>-58.364566</v>
+      </c>
+      <c r="N85" t="n">
+        <v>-34.639404</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-08 13:28:10)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P389"/>
+  <dimension ref="A1:P390"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29901,6 +29901,82 @@
         </is>
       </c>
       <c r="P389" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>-585</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>9/8/2025</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>Rio Cuarto 3267</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>Pendente ADM</t>
+        </is>
+      </c>
+      <c r="F390" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G390" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H390" t="inlineStr">
+        <is>
+          <t>Desmonte de columna</t>
+        </is>
+      </c>
+      <c r="I390" t="n">
+        <v>1</v>
+      </c>
+      <c r="J390" t="inlineStr">
+        <is>
+          <t>Desmonte</t>
+        </is>
+      </c>
+      <c r="K390" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L390" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M390" t="n">
+        <v>-58.39368</v>
+      </c>
+      <c r="N390" t="n">
+        <v>-34.652663</v>
+      </c>
+      <c r="O390" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P390" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
@@ -29917,7 +29993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P90"/>
+  <dimension ref="A1:P91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36726,6 +36802,82 @@
         </is>
       </c>
       <c r="P90" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>-585</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>9/8/2025</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Rio Cuarto 3267</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Pendente ADM</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Desmonte de columna</t>
+        </is>
+      </c>
+      <c r="I91" t="n">
+        <v>1</v>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>Desmonte</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M91" t="n">
+        <v>-58.39368</v>
+      </c>
+      <c r="N91" t="n">
+        <v>-34.652663</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-10 08:42:26)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P394"/>
+  <dimension ref="A1:P393"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25889,32 +25889,32 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>-560</t>
+          <t>5503</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/22/2025</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>Pinzon 1590</t>
+          <t>CRAMER AV. 1771</t>
         </is>
       </c>
       <c r="D337" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E337" t="inlineStr">
         <is>
-          <t>809098712</t>
+          <t>809102564</t>
         </is>
       </c>
       <c r="F337" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G337" t="inlineStr">
@@ -25924,7 +25924,7 @@
       </c>
       <c r="H337" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I337" t="n">
@@ -25946,46 +25946,46 @@
         </is>
       </c>
       <c r="M337" t="n">
-        <v>-58.373506</v>
+        <v>-58.458506</v>
       </c>
       <c r="N337" t="n">
-        <v>-34.63706</v>
+        <v>-34.56783</v>
       </c>
       <c r="O337" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P337" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>5503</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>8/22/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>CRAMER AV. 1771</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>809102564</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
@@ -26000,7 +26000,7 @@
       </c>
       <c r="H338" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I338" t="n">
@@ -26022,10 +26022,10 @@
         </is>
       </c>
       <c r="M338" t="n">
-        <v>-58.458506</v>
+        <v>-58.472869</v>
       </c>
       <c r="N338" t="n">
-        <v>-34.56783</v>
+        <v>-34.562</v>
       </c>
       <c r="O338" t="inlineStr">
         <is>
@@ -26041,7 +26041,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>7080</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
@@ -26051,17 +26051,17 @@
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>UGARTE, MANUEL 2196</t>
         </is>
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>809125906</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
@@ -26098,14 +26098,14 @@
         </is>
       </c>
       <c r="M339" t="n">
-        <v>-58.472869</v>
+        <v>-58.459402</v>
       </c>
       <c r="N339" t="n">
-        <v>-34.562</v>
+        <v>-34.555262</v>
       </c>
       <c r="O339" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P339" t="inlineStr">
@@ -26117,7 +26117,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>7080</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -26127,22 +26127,22 @@
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 2196</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>809125906</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G340" t="inlineStr">
@@ -26152,7 +26152,7 @@
       </c>
       <c r="H340" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada mismo caso que 7083</t>
         </is>
       </c>
       <c r="I340" t="n">
@@ -26174,26 +26174,26 @@
         </is>
       </c>
       <c r="M340" t="n">
-        <v>-58.459402</v>
+        <v>-58.402244</v>
       </c>
       <c r="N340" t="n">
-        <v>-34.555262</v>
+        <v>-34.619401</v>
       </c>
       <c r="O340" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P340" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>7021</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
@@ -26203,22 +26203,22 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>VERA 445</t>
         </is>
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E341" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809155622</t>
         </is>
       </c>
       <c r="F341" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G341" t="inlineStr">
@@ -26228,7 +26228,7 @@
       </c>
       <c r="H341" t="inlineStr">
         <is>
-          <t>Picada mismo caso que 7083</t>
+          <t>Correrla para sacarla del cantero</t>
         </is>
       </c>
       <c r="I341" t="n">
@@ -26250,14 +26250,14 @@
         </is>
       </c>
       <c r="M341" t="n">
-        <v>-58.402244</v>
+        <v>-58.437181</v>
       </c>
       <c r="N341" t="n">
-        <v>-34.619401</v>
+        <v>-34.5995</v>
       </c>
       <c r="O341" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P341" t="inlineStr">
@@ -26269,7 +26269,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>7021</t>
+          <t>809156751</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -26279,22 +26279,22 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>VERA 445</t>
+          <t>Av San Martín 5045</t>
         </is>
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E342" t="inlineStr">
         <is>
-          <t>809155622</t>
+          <t>809156751</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>Sin Asignar</t>
         </is>
       </c>
       <c r="G342" t="inlineStr">
@@ -26304,11 +26304,11 @@
       </c>
       <c r="H342" t="inlineStr">
         <is>
-          <t>Correrla para sacarla del cantero</t>
+          <t>aplomar o cambiar poste de 11 con rienda a pique</t>
         </is>
       </c>
       <c r="I342" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J342" t="inlineStr">
         <is>
@@ -26322,30 +26322,30 @@
       </c>
       <c r="L342" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M342" t="n">
-        <v>-58.437181</v>
+        <v>-58.489141</v>
       </c>
       <c r="N342" t="n">
-        <v>-34.5995</v>
+        <v>-34.597221</v>
       </c>
       <c r="O342" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P342" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>809156751</t>
+          <t>7149</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
@@ -26355,22 +26355,22 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>Av San Martín 5045</t>
+          <t>QUITO 3666</t>
         </is>
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E343" t="inlineStr">
         <is>
-          <t>809156751</t>
+          <t>809168441</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>Sin Asignar</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G343" t="inlineStr">
@@ -26380,11 +26380,11 @@
       </c>
       <c r="H343" t="inlineStr">
         <is>
-          <t>aplomar o cambiar poste de 11 con rienda a pique</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I343" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J343" t="inlineStr">
         <is>
@@ -26398,30 +26398,30 @@
       </c>
       <c r="L343" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M343" t="n">
-        <v>-58.489141</v>
+        <v>-58.41791</v>
       </c>
       <c r="N343" t="n">
-        <v>-34.597221</v>
+        <v>-34.616706</v>
       </c>
       <c r="O343" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P343" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>7149</t>
+          <t>-565</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
@@ -26431,7 +26431,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>QUITO 3666</t>
+          <t>Venezuela 3888</t>
         </is>
       </c>
       <c r="D344" t="inlineStr">
@@ -26441,12 +26441,12 @@
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>809168441</t>
+          <t>809168446</t>
         </is>
       </c>
       <c r="F344" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>Sin Asignar</t>
         </is>
       </c>
       <c r="G344" t="inlineStr">
@@ -26456,7 +26456,7 @@
       </c>
       <c r="H344" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I344" t="n">
@@ -26478,10 +26478,10 @@
         </is>
       </c>
       <c r="M344" t="n">
-        <v>-58.41791</v>
+        <v>-58.420309</v>
       </c>
       <c r="N344" t="n">
-        <v>-34.616706</v>
+        <v>-34.61767</v>
       </c>
       <c r="O344" t="inlineStr">
         <is>
@@ -26497,32 +26497,32 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>-565</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>Venezuela 3888</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E345" t="inlineStr">
         <is>
-          <t>809168446</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>Sin Asignar</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G345" t="inlineStr">
@@ -26532,7 +26532,7 @@
       </c>
       <c r="H345" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I345" t="n">
@@ -26554,10 +26554,10 @@
         </is>
       </c>
       <c r="M345" t="n">
-        <v>-58.420309</v>
+        <v>-58.393882</v>
       </c>
       <c r="N345" t="n">
-        <v>-34.61767</v>
+        <v>-34.604721</v>
       </c>
       <c r="O345" t="inlineStr">
         <is>
@@ -26573,7 +26573,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
@@ -26583,7 +26583,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D346" t="inlineStr">
@@ -26593,7 +26593,7 @@
       </c>
       <c r="E346" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F346" t="inlineStr">
@@ -26630,14 +26630,14 @@
         </is>
       </c>
       <c r="M346" t="n">
-        <v>-58.393882</v>
+        <v>-58.394543</v>
       </c>
       <c r="N346" t="n">
-        <v>-34.604721</v>
+        <v>-34.620732</v>
       </c>
       <c r="O346" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P346" t="inlineStr">
@@ -26649,7 +26649,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
@@ -26659,17 +26659,17 @@
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E347" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F347" t="inlineStr">
@@ -26702,18 +26702,18 @@
       </c>
       <c r="L347" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M347" t="n">
-        <v>-58.394543</v>
+        <v>-58.427206</v>
       </c>
       <c r="N347" t="n">
-        <v>-34.620732</v>
+        <v>-34.602914</v>
       </c>
       <c r="O347" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P347" t="inlineStr">
@@ -26725,7 +26725,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>7050</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
@@ -26735,17 +26735,17 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>PRINGLES 788</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E348" t="inlineStr">
         <is>
-          <t>809195664</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
@@ -26755,12 +26755,12 @@
       </c>
       <c r="G348" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H348" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I348" t="n">
@@ -26773,7 +26773,7 @@
       </c>
       <c r="K348" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L348" t="inlineStr">
@@ -26782,14 +26782,14 @@
         </is>
       </c>
       <c r="M348" t="n">
-        <v>-58.427206</v>
+        <v>-58.435017</v>
       </c>
       <c r="N348" t="n">
-        <v>-34.602914</v>
+        <v>-34.622044</v>
       </c>
       <c r="O348" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P348" t="inlineStr">
@@ -26801,17 +26801,17 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>7064</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>GAONA AV. 1189</t>
         </is>
       </c>
       <c r="D349" t="inlineStr">
@@ -26821,7 +26821,7 @@
       </c>
       <c r="E349" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809257408</t>
         </is>
       </c>
       <c r="F349" t="inlineStr">
@@ -26831,12 +26831,12 @@
       </c>
       <c r="G349" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H349" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
         </is>
       </c>
       <c r="I349" t="n">
@@ -26849,7 +26849,7 @@
       </c>
       <c r="K349" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L349" t="inlineStr">
@@ -26858,14 +26858,14 @@
         </is>
       </c>
       <c r="M349" t="n">
-        <v>-58.435017</v>
+        <v>-58.446008</v>
       </c>
       <c r="N349" t="n">
-        <v>-34.622044</v>
+        <v>-34.607602</v>
       </c>
       <c r="O349" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P349" t="inlineStr">
@@ -26877,32 +26877,32 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>7064</t>
+          <t>-569</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>GAONA AV. 1189</t>
+          <t>Palpa 2862</t>
         </is>
       </c>
       <c r="D350" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E350" t="inlineStr">
         <is>
-          <t>809257408</t>
+          <t>809257759</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G350" t="inlineStr">
@@ -26912,7 +26912,7 @@
       </c>
       <c r="H350" t="inlineStr">
         <is>
-          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I350" t="n">
@@ -26930,30 +26930,30 @@
       </c>
       <c r="L350" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M350" t="n">
-        <v>-58.446008</v>
+        <v>-58.449512</v>
       </c>
       <c r="N350" t="n">
-        <v>-34.607602</v>
+        <v>-34.573404</v>
       </c>
       <c r="O350" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P350" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>-569</t>
+          <t>7157</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
@@ -26963,22 +26963,22 @@
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>Palpa 2862</t>
+          <t>CALVO, CARLOS 1750</t>
         </is>
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E351" t="inlineStr">
         <is>
-          <t>809257759</t>
+          <t>809257762</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G351" t="inlineStr">
@@ -27010,26 +27010,26 @@
         </is>
       </c>
       <c r="M351" t="n">
-        <v>-58.449512</v>
+        <v>-58.390806</v>
       </c>
       <c r="N351" t="n">
-        <v>-34.573404</v>
+        <v>-34.620213</v>
       </c>
       <c r="O351" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P351" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>7157</t>
+          <t>-571</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
@@ -27039,22 +27039,22 @@
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 1750</t>
+          <t>Alberti 1603</t>
         </is>
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E352" t="inlineStr">
         <is>
-          <t>809257762</t>
+          <t>809257763</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>Sin Asignar</t>
         </is>
       </c>
       <c r="G352" t="inlineStr">
@@ -27086,10 +27086,10 @@
         </is>
       </c>
       <c r="M352" t="n">
-        <v>-58.390806</v>
+        <v>-58.39992</v>
       </c>
       <c r="N352" t="n">
-        <v>-34.620213</v>
+        <v>-34.628742</v>
       </c>
       <c r="O352" t="inlineStr">
         <is>
@@ -27105,7 +27105,7 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>-571</t>
+          <t>-572</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
@@ -27115,7 +27115,7 @@
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>Alberti 1603</t>
+          <t>JUJUY 1633</t>
         </is>
       </c>
       <c r="D353" t="inlineStr">
@@ -27125,7 +27125,7 @@
       </c>
       <c r="E353" t="inlineStr">
         <is>
-          <t>809257763</t>
+          <t>809257764</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
@@ -27162,10 +27162,10 @@
         </is>
       </c>
       <c r="M353" t="n">
-        <v>-58.39992</v>
+        <v>-58.401125</v>
       </c>
       <c r="N353" t="n">
-        <v>-34.628742</v>
+        <v>-34.629165</v>
       </c>
       <c r="O353" t="inlineStr">
         <is>
@@ -27181,17 +27181,17 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>-572</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>JUJUY 1633</t>
+          <t>HERRERA 1998</t>
         </is>
       </c>
       <c r="D354" t="inlineStr">
@@ -27201,12 +27201,12 @@
       </c>
       <c r="E354" t="inlineStr">
         <is>
-          <t>809257764</t>
+          <t>809268244</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
         <is>
-          <t>Sin Asignar</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G354" t="inlineStr">
@@ -27216,7 +27216,7 @@
       </c>
       <c r="H354" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I354" t="n">
@@ -27234,14 +27234,14 @@
       </c>
       <c r="L354" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M354" t="n">
-        <v>-58.401125</v>
+        <v>-58.37456</v>
       </c>
       <c r="N354" t="n">
-        <v>-34.629165</v>
+        <v>-34.649779</v>
       </c>
       <c r="O354" t="inlineStr">
         <is>
@@ -27257,7 +27257,7 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>6465</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
@@ -27267,22 +27267,22 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>AGUIRRE 368</t>
         </is>
       </c>
       <c r="D355" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>809268249</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G355" t="inlineStr">
@@ -27292,7 +27292,7 @@
       </c>
       <c r="H355" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I355" t="n">
@@ -27310,18 +27310,18 @@
       </c>
       <c r="L355" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M355" t="n">
-        <v>-58.37456</v>
+        <v>-58.434651</v>
       </c>
       <c r="N355" t="n">
-        <v>-34.649779</v>
+        <v>-34.598814</v>
       </c>
       <c r="O355" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P355" t="inlineStr">
@@ -27333,7 +27333,7 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>6465</t>
+          <t>7095</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
@@ -27343,7 +27343,7 @@
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>AGUIRRE 368</t>
+          <t>SAN MARTIN AV. 4515</t>
         </is>
       </c>
       <c r="D356" t="inlineStr">
@@ -27353,7 +27353,7 @@
       </c>
       <c r="E356" t="inlineStr">
         <is>
-          <t>809268249</t>
+          <t>809268240</t>
         </is>
       </c>
       <c r="F356" t="inlineStr">
@@ -27368,7 +27368,7 @@
       </c>
       <c r="H356" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna chocada</t>
         </is>
       </c>
       <c r="I356" t="n">
@@ -27386,30 +27386,30 @@
       </c>
       <c r="L356" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M356" t="n">
-        <v>-58.434651</v>
+        <v>-58.483415</v>
       </c>
       <c r="N356" t="n">
-        <v>-34.598814</v>
+        <v>-34.597663</v>
       </c>
       <c r="O356" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P356" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>7095</t>
+          <t>-573</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
@@ -27419,22 +27419,22 @@
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>SAN MARTIN AV. 4515</t>
+          <t>Juramento 5211</t>
         </is>
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E357" t="inlineStr">
         <is>
-          <t>809268240</t>
+          <t>809268259</t>
         </is>
       </c>
       <c r="F357" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>Sin Asignar</t>
         </is>
       </c>
       <c r="G357" t="inlineStr">
@@ -27444,7 +27444,7 @@
       </c>
       <c r="H357" t="inlineStr">
         <is>
-          <t>Columna chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I357" t="n">
@@ -27462,14 +27462,14 @@
       </c>
       <c r="L357" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M357" t="n">
-        <v>-58.483415</v>
+        <v>-58.484108</v>
       </c>
       <c r="N357" t="n">
-        <v>-34.597663</v>
+        <v>-34.579014</v>
       </c>
       <c r="O357" t="inlineStr">
         <is>
@@ -27485,7 +27485,7 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>-573</t>
+          <t>7171</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
@@ -27495,7 +27495,7 @@
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>Juramento 5211</t>
+          <t>OLAZABAL AV. 5531</t>
         </is>
       </c>
       <c r="D358" t="inlineStr">
@@ -27505,12 +27505,12 @@
       </c>
       <c r="E358" t="inlineStr">
         <is>
-          <t>809268259</t>
+          <t>809268253</t>
         </is>
       </c>
       <c r="F358" t="inlineStr">
         <is>
-          <t>Sin Asignar</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G358" t="inlineStr">
@@ -27542,10 +27542,10 @@
         </is>
       </c>
       <c r="M358" t="n">
-        <v>-58.484108</v>
+        <v>-58.491028</v>
       </c>
       <c r="N358" t="n">
-        <v>-34.579014</v>
+        <v>-34.579381</v>
       </c>
       <c r="O358" t="inlineStr">
         <is>
@@ -27561,27 +27561,27 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>7171</t>
+          <t>7089</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>OLAZABAL AV. 5531</t>
+          <t>SAN ANTONIO 637</t>
         </is>
       </c>
       <c r="D359" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E359" t="inlineStr">
         <is>
-          <t>809268253</t>
+          <t>809270751</t>
         </is>
       </c>
       <c r="F359" t="inlineStr">
@@ -27596,7 +27596,7 @@
       </c>
       <c r="H359" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I359" t="n">
@@ -27618,36 +27618,36 @@
         </is>
       </c>
       <c r="M359" t="n">
-        <v>-58.491028</v>
+        <v>-58.37805</v>
       </c>
       <c r="N359" t="n">
-        <v>-34.579381</v>
+        <v>-34.649722</v>
       </c>
       <c r="O359" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P359" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>7089</t>
+          <t>7090</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 637</t>
+          <t>SAN ANTONIO 625</t>
         </is>
       </c>
       <c r="D360" t="inlineStr">
@@ -27657,7 +27657,7 @@
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t>809270751</t>
+          <t>809270753</t>
         </is>
       </c>
       <c r="F360" t="inlineStr">
@@ -27694,10 +27694,10 @@
         </is>
       </c>
       <c r="M360" t="n">
-        <v>-58.37805</v>
+        <v>-58.378104</v>
       </c>
       <c r="N360" t="n">
-        <v>-34.649722</v>
+        <v>-34.649578</v>
       </c>
       <c r="O360" t="inlineStr">
         <is>
@@ -27713,7 +27713,7 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>7091</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
@@ -27723,7 +27723,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 625</t>
+          <t>SUAREZ AV. 1966</t>
         </is>
       </c>
       <c r="D361" t="inlineStr">
@@ -27733,7 +27733,7 @@
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>809270753</t>
+          <t>809279022</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
@@ -27770,10 +27770,10 @@
         </is>
       </c>
       <c r="M361" t="n">
-        <v>-58.378104</v>
+        <v>-58.377974</v>
       </c>
       <c r="N361" t="n">
-        <v>-34.649578</v>
+        <v>-34.641024</v>
       </c>
       <c r="O361" t="inlineStr">
         <is>
@@ -27789,7 +27789,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>7091</t>
+          <t>7096</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
@@ -27799,17 +27799,17 @@
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>SUAREZ AV. 1966</t>
+          <t>VEDIA, AGUSTIN DE 2185</t>
         </is>
       </c>
       <c r="D362" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E362" t="inlineStr">
         <is>
-          <t>809279022</t>
+          <t>809279069</t>
         </is>
       </c>
       <c r="F362" t="inlineStr">
@@ -27846,14 +27846,14 @@
         </is>
       </c>
       <c r="M362" t="n">
-        <v>-58.377974</v>
+        <v>-58.435511</v>
       </c>
       <c r="N362" t="n">
-        <v>-34.641024</v>
+        <v>-34.644702</v>
       </c>
       <c r="O362" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P362" t="inlineStr">
@@ -27865,7 +27865,7 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>7096</t>
+          <t>7097</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
@@ -27875,7 +27875,7 @@
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
         </is>
       </c>
       <c r="D363" t="inlineStr">
@@ -27885,12 +27885,12 @@
       </c>
       <c r="E363" t="inlineStr">
         <is>
-          <t>809279069</t>
+          <t>809279093</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G363" t="inlineStr">
@@ -27900,7 +27900,7 @@
       </c>
       <c r="H363" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I363" t="n">
@@ -27918,14 +27918,14 @@
       </c>
       <c r="L363" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M363" t="n">
-        <v>-58.435511</v>
+        <v>-58.458659</v>
       </c>
       <c r="N363" t="n">
-        <v>-34.644702</v>
+        <v>-34.630464</v>
       </c>
       <c r="O363" t="inlineStr">
         <is>
@@ -27941,7 +27941,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>7097</t>
+          <t>-575</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
@@ -27951,22 +27951,22 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
+          <t>Amenabar 3064</t>
         </is>
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>809279093</t>
+          <t>809281299</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G364" t="inlineStr">
@@ -27994,65 +27994,65 @@
       </c>
       <c r="L364" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M364" t="n">
-        <v>-58.458659</v>
+        <v>-58.465984</v>
       </c>
       <c r="N364" t="n">
-        <v>-34.630464</v>
+        <v>-34.554869</v>
       </c>
       <c r="O364" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P364" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>-575</t>
+          <t>4698</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>Amenabar 3064</t>
+          <t>REPETTO, NICOLAS, DR. 93</t>
         </is>
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E365" t="inlineStr">
         <is>
-          <t>809281299</t>
+          <t>ICD30593982</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G365" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H365" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
         </is>
       </c>
       <c r="I365" t="n">
@@ -28065,45 +28065,45 @@
       </c>
       <c r="K365" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L365" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M365" t="n">
-        <v>-58.465984</v>
+        <v>-58.443232</v>
       </c>
       <c r="N365" t="n">
-        <v>-34.554869</v>
+        <v>-34.620007</v>
       </c>
       <c r="O365" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P365" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>4698</t>
+          <t>7102</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/30/2025</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
+          <t>AMBERES 995</t>
         </is>
       </c>
       <c r="D366" t="inlineStr">
@@ -28113,7 +28113,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>ICD30593982</t>
+          <t>809309598</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
@@ -28123,12 +28123,12 @@
       </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H366" t="inlineStr">
         <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I366" t="n">
@@ -28141,19 +28141,19 @@
       </c>
       <c r="K366" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L366" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M366" t="n">
-        <v>-58.443232</v>
+        <v>-58.453382</v>
       </c>
       <c r="N366" t="n">
-        <v>-34.620007</v>
+        <v>-34.612707</v>
       </c>
       <c r="O366" t="inlineStr">
         <is>
@@ -28169,32 +28169,32 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>7102</t>
+          <t>-576</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>8/30/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>AMBERES 995</t>
+          <t>Av. Boyacá 2030</t>
         </is>
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E367" t="inlineStr">
         <is>
-          <t>809309598</t>
+          <t>809309606</t>
         </is>
       </c>
       <c r="F367" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G367" t="inlineStr">
@@ -28226,46 +28226,46 @@
         </is>
       </c>
       <c r="M367" t="n">
-        <v>-58.453382</v>
+        <v>-58.471173</v>
       </c>
       <c r="N367" t="n">
-        <v>-34.612707</v>
+        <v>-34.60704</v>
       </c>
       <c r="O367" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P367" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>-576</t>
+          <t>7111</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>Av. Boyacá 2030</t>
+          <t>VILELA 3699</t>
         </is>
       </c>
       <c r="D368" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>809309606</t>
+          <t>809371823</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
@@ -28280,7 +28280,7 @@
       </c>
       <c r="H368" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I368" t="n">
@@ -28298,18 +28298,18 @@
       </c>
       <c r="L368" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M368" t="n">
-        <v>-58.471173</v>
+        <v>-58.482817</v>
       </c>
       <c r="N368" t="n">
-        <v>-34.60704</v>
+        <v>-34.550845</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P368" t="inlineStr">
@@ -28321,7 +28321,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>7111</t>
+          <t>7112</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
@@ -28331,22 +28331,22 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>VILELA 3699</t>
+          <t>OLLEROS 2488</t>
         </is>
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E369" t="inlineStr">
         <is>
-          <t>809371823</t>
+          <t>809371829</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G369" t="inlineStr">
@@ -28378,51 +28378,51 @@
         </is>
       </c>
       <c r="M369" t="n">
-        <v>-58.482817</v>
+        <v>-58.444214</v>
       </c>
       <c r="N369" t="n">
-        <v>-34.550845</v>
+        <v>-34.571197</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P369" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>7112</t>
+          <t>7118</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>OLLEROS 2488</t>
+          <t>CUBAS, JOSE 2211</t>
         </is>
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E370" t="inlineStr">
         <is>
-          <t>809371829</t>
+          <t>809406168</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G370" t="inlineStr">
@@ -28432,7 +28432,7 @@
       </c>
       <c r="H370" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I370" t="n">
@@ -28450,30 +28450,30 @@
       </c>
       <c r="L370" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M370" t="n">
-        <v>-58.444214</v>
+        <v>-58.492448</v>
       </c>
       <c r="N370" t="n">
-        <v>-34.571197</v>
+        <v>-34.58372</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P370" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>7118</t>
+          <t>7120</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -28483,7 +28483,7 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>CUBAS, JOSE 2211</t>
+          <t>BLANCO ENCALADA 4210</t>
         </is>
       </c>
       <c r="D371" t="inlineStr">
@@ -28493,12 +28493,12 @@
       </c>
       <c r="E371" t="inlineStr">
         <is>
-          <t>809406168</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G371" t="inlineStr">
@@ -28508,7 +28508,7 @@
       </c>
       <c r="H371" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I371" t="n">
@@ -28521,7 +28521,7 @@
       </c>
       <c r="K371" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L371" t="inlineStr">
@@ -28530,14 +28530,14 @@
         </is>
       </c>
       <c r="M371" t="n">
-        <v>-58.492448</v>
+        <v>-58.477593</v>
       </c>
       <c r="N371" t="n">
-        <v>-34.58372</v>
+        <v>-34.570321</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P371" t="inlineStr">
@@ -28549,7 +28549,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>7120</t>
+          <t>-577</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
@@ -28559,22 +28559,22 @@
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>BLANCO ENCALADA 4210</t>
+          <t>Manuel Ugarte 2318</t>
         </is>
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E372" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809406177</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G372" t="inlineStr">
@@ -28584,7 +28584,7 @@
       </c>
       <c r="H372" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir traspaso de fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I372" t="n">
@@ -28597,7 +28597,7 @@
       </c>
       <c r="K372" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L372" t="inlineStr">
@@ -28606,14 +28606,14 @@
         </is>
       </c>
       <c r="M372" t="n">
-        <v>-58.477593</v>
+        <v>-58.460635</v>
       </c>
       <c r="N372" t="n">
-        <v>-34.570321</v>
+        <v>-34.555932</v>
       </c>
       <c r="O372" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P372" t="inlineStr">
@@ -28625,7 +28625,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>-577</t>
+          <t>-578</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
@@ -28635,7 +28635,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>Manuel Ugarte 2318</t>
+          <t>Pedro I Rivera 2536</t>
         </is>
       </c>
       <c r="D373" t="inlineStr">
@@ -28645,7 +28645,7 @@
       </c>
       <c r="E373" t="inlineStr">
         <is>
-          <t>809406177</t>
+          <t>809406189</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
@@ -28682,10 +28682,10 @@
         </is>
       </c>
       <c r="M373" t="n">
-        <v>-58.460635</v>
+        <v>-58.462327</v>
       </c>
       <c r="N373" t="n">
-        <v>-34.555932</v>
+        <v>-34.557565</v>
       </c>
       <c r="O373" t="inlineStr">
         <is>
@@ -28701,7 +28701,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>-578</t>
+          <t>-579</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -28711,7 +28711,7 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>Pedro I Rivera 2536</t>
+          <t>Pedro Rivera 2546</t>
         </is>
       </c>
       <c r="D374" t="inlineStr">
@@ -28721,7 +28721,7 @@
       </c>
       <c r="E374" t="inlineStr">
         <is>
-          <t>809406189</t>
+          <t>ICD30612785</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
@@ -28736,7 +28736,7 @@
       </c>
       <c r="H374" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R200 para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I374" t="n">
@@ -28749,7 +28749,7 @@
       </c>
       <c r="K374" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L374" t="inlineStr">
@@ -28758,10 +28758,10 @@
         </is>
       </c>
       <c r="M374" t="n">
-        <v>-58.462327</v>
+        <v>-58.462479</v>
       </c>
       <c r="N374" t="n">
-        <v>-34.557565</v>
+        <v>-34.55765</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -28777,32 +28777,32 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>-579</t>
+          <t>-580</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/3/2025</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>Pedro Rivera 2546</t>
+          <t>Av Nazca 3985</t>
         </is>
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t>ICD30612785</t>
+          <t>809409491</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>Sin Asignar</t>
         </is>
       </c>
       <c r="G375" t="inlineStr">
@@ -28812,7 +28812,7 @@
       </c>
       <c r="H375" t="inlineStr">
         <is>
-          <t>Colocar R200 para pedir traspaso de equipos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I375" t="n">
@@ -28825,7 +28825,7 @@
       </c>
       <c r="K375" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L375" t="inlineStr">
@@ -28834,14 +28834,14 @@
         </is>
       </c>
       <c r="M375" t="n">
-        <v>-58.462479</v>
+        <v>-58.497366</v>
       </c>
       <c r="N375" t="n">
-        <v>-34.55765</v>
+        <v>-34.591544</v>
       </c>
       <c r="O375" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P375" t="inlineStr">
@@ -28853,7 +28853,7 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>-580</t>
+          <t>7136</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
@@ -28863,7 +28863,7 @@
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>Av Nazca 3985</t>
+          <t>FERRARI 455</t>
         </is>
       </c>
       <c r="D376" t="inlineStr">
@@ -28873,12 +28873,12 @@
       </c>
       <c r="E376" t="inlineStr">
         <is>
-          <t>809409491</t>
+          <t>809427020</t>
         </is>
       </c>
       <c r="F376" t="inlineStr">
         <is>
-          <t>Sin Asignar</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G376" t="inlineStr">
@@ -28906,14 +28906,14 @@
       </c>
       <c r="L376" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M376" t="n">
-        <v>-58.497366</v>
+        <v>-58.441587</v>
       </c>
       <c r="N376" t="n">
-        <v>-34.591544</v>
+        <v>-34.60547</v>
       </c>
       <c r="O376" t="inlineStr">
         <is>
@@ -28929,7 +28929,7 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>7136</t>
+          <t>7150</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
@@ -28939,17 +28939,17 @@
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>FERRARI 455</t>
+          <t>Bartolomé Mitre 3070</t>
         </is>
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E377" t="inlineStr">
         <is>
-          <t>809427020</t>
+          <t>809427021</t>
         </is>
       </c>
       <c r="F377" t="inlineStr">
@@ -28964,7 +28964,7 @@
       </c>
       <c r="H377" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I377" t="n">
@@ -28982,55 +28982,51 @@
       </c>
       <c r="L377" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M377" t="n">
-        <v>-58.441587</v>
+        <v>-58.410025</v>
       </c>
       <c r="N377" t="n">
-        <v>-34.60547</v>
+        <v>-34.609184</v>
       </c>
       <c r="O377" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P377" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>7150</t>
+          <t>-581</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>9/3/2025</t>
+          <t>9/4/2025</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>Bartolomé Mitre 3070</t>
-        </is>
-      </c>
-      <c r="D378" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+          <t>Praga 1380</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr"/>
       <c r="E378" t="inlineStr">
         <is>
-          <t>809427021</t>
+          <t>809432814</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G378" t="inlineStr">
@@ -29044,7 +29040,7 @@
         </is>
       </c>
       <c r="I378" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J378" t="inlineStr">
         <is>
@@ -29062,42 +29058,46 @@
         </is>
       </c>
       <c r="M378" t="n">
-        <v>-58.410025</v>
+        <v>-58.481608</v>
       </c>
       <c r="N378" t="n">
-        <v>-34.609184</v>
+        <v>-34.587837</v>
       </c>
       <c r="O378" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P378" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>-581</t>
+          <t>7169</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>9/4/2025</t>
+          <t>9/5/2025</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>Praga 1380</t>
-        </is>
-      </c>
-      <c r="D379" t="inlineStr"/>
+          <t>SAN NICOLAS 5045</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
       <c r="E379" t="inlineStr">
         <is>
-          <t>809432814</t>
+          <t>809492980</t>
         </is>
       </c>
       <c r="F379" t="inlineStr">
@@ -29112,11 +29112,11 @@
       </c>
       <c r="H379" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Poste quebrado</t>
         </is>
       </c>
       <c r="I379" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J379" t="inlineStr">
         <is>
@@ -29130,14 +29130,14 @@
       </c>
       <c r="L379" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M379" t="n">
-        <v>-58.481608</v>
+        <v>-58.515637</v>
       </c>
       <c r="N379" t="n">
-        <v>-34.587837</v>
+        <v>-34.589993</v>
       </c>
       <c r="O379" t="inlineStr">
         <is>
@@ -29153,27 +29153,27 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>7169</t>
+          <t>-583</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>9/5/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5045</t>
+          <t>Av Eva Perón 1145</t>
         </is>
       </c>
       <c r="D380" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E380" t="inlineStr">
         <is>
-          <t>809492980</t>
+          <t>809504290</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
@@ -29188,7 +29188,7 @@
       </c>
       <c r="H380" t="inlineStr">
         <is>
-          <t>Poste quebrado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I380" t="n">
@@ -29206,30 +29206,30 @@
       </c>
       <c r="L380" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M380" t="n">
-        <v>-58.515637</v>
+        <v>-58.441547</v>
       </c>
       <c r="N380" t="n">
-        <v>-34.589993</v>
+        <v>-34.630481</v>
       </c>
       <c r="O380" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P380" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>-583</t>
+          <t>-585</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
@@ -29239,22 +29239,22 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>Av Eva Perón 1145</t>
+          <t>Rio Cuarto 3267</t>
         </is>
       </c>
       <c r="D381" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E381" t="inlineStr">
         <is>
-          <t>809504290</t>
+          <t>ICD30704450</t>
         </is>
       </c>
       <c r="F381" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G381" t="inlineStr">
@@ -29264,7 +29264,7 @@
       </c>
       <c r="H381" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmonte de columna</t>
         </is>
       </c>
       <c r="I381" t="n">
@@ -29272,7 +29272,7 @@
       </c>
       <c r="J381" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K381" t="inlineStr">
@@ -29282,18 +29282,18 @@
       </c>
       <c r="L381" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M381" t="n">
-        <v>-58.441547</v>
+        <v>-58.39368</v>
       </c>
       <c r="N381" t="n">
-        <v>-34.630481</v>
+        <v>-34.652663</v>
       </c>
       <c r="O381" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P381" t="inlineStr">
@@ -29305,7 +29305,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>-585</t>
+          <t>7174</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
@@ -29315,22 +29315,22 @@
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>Rio Cuarto 3267</t>
+          <t>FERNANDEZ BLANCO 2320</t>
         </is>
       </c>
       <c r="D382" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E382" t="inlineStr">
         <is>
-          <t>ICD30704450</t>
+          <t>809526154</t>
         </is>
       </c>
       <c r="F382" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G382" t="inlineStr">
@@ -29340,7 +29340,7 @@
       </c>
       <c r="H382" t="inlineStr">
         <is>
-          <t>Desmonte de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I382" t="n">
@@ -29348,7 +29348,7 @@
       </c>
       <c r="J382" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K382" t="inlineStr">
@@ -29358,30 +29358,30 @@
       </c>
       <c r="L382" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M382" t="n">
-        <v>-58.39368</v>
+        <v>-58.481983</v>
       </c>
       <c r="N382" t="n">
-        <v>-34.652663</v>
+        <v>-34.573931</v>
       </c>
       <c r="O382" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P382" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>7174</t>
+          <t>7177</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -29391,7 +29391,7 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>FERNANDEZ BLANCO 2320</t>
+          <t>LUGONES 2830</t>
         </is>
       </c>
       <c r="D383" t="inlineStr">
@@ -29401,7 +29401,7 @@
       </c>
       <c r="E383" t="inlineStr">
         <is>
-          <t>809526154</t>
+          <t>809526156</t>
         </is>
       </c>
       <c r="F383" t="inlineStr">
@@ -29438,10 +29438,10 @@
         </is>
       </c>
       <c r="M383" t="n">
-        <v>-58.481983</v>
+        <v>-58.482786</v>
       </c>
       <c r="N383" t="n">
-        <v>-34.573931</v>
+        <v>-34.56748</v>
       </c>
       <c r="O383" t="inlineStr">
         <is>
@@ -29457,7 +29457,7 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>7177</t>
+          <t>7180</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
@@ -29467,22 +29467,22 @@
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>LUGONES 2830</t>
+          <t>GORRITI 4417</t>
         </is>
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E384" t="inlineStr">
         <is>
-          <t>809526156</t>
+          <t>809526157</t>
         </is>
       </c>
       <c r="F384" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G384" t="inlineStr">
@@ -29514,26 +29514,26 @@
         </is>
       </c>
       <c r="M384" t="n">
-        <v>-58.482786</v>
+        <v>-58.425358</v>
       </c>
       <c r="N384" t="n">
-        <v>-34.56748</v>
+        <v>-34.593308</v>
       </c>
       <c r="O384" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P384" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>7180</t>
+          <t>7184</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
@@ -29543,22 +29543,22 @@
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>GORRITI 4417</t>
+          <t>VALLEJOS 2221</t>
         </is>
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E385" t="inlineStr">
         <is>
-          <t>809526157</t>
+          <t>809526160</t>
         </is>
       </c>
       <c r="F385" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G385" t="inlineStr">
@@ -29590,26 +29590,26 @@
         </is>
       </c>
       <c r="M385" t="n">
-        <v>-58.425358</v>
+        <v>-58.493225</v>
       </c>
       <c r="N385" t="n">
-        <v>-34.593308</v>
+        <v>-34.583095</v>
       </c>
       <c r="O385" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P385" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>7184</t>
+          <t>7186</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
@@ -29619,22 +29619,22 @@
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>VALLEJOS 2221</t>
+          <t>NICARAGUA 5510</t>
         </is>
       </c>
       <c r="D386" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E386" t="inlineStr">
         <is>
-          <t>809526160</t>
+          <t>809526162</t>
         </is>
       </c>
       <c r="F386" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G386" t="inlineStr">
@@ -29666,26 +29666,26 @@
         </is>
       </c>
       <c r="M386" t="n">
-        <v>-58.493225</v>
+        <v>-58.432726</v>
       </c>
       <c r="N386" t="n">
-        <v>-34.583095</v>
+        <v>-34.582328</v>
       </c>
       <c r="O386" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P386" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>7186</t>
+          <t>7194</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
@@ -29695,17 +29695,17 @@
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>NICARAGUA 5510</t>
+          <t>CASEROS AV. 2032</t>
         </is>
       </c>
       <c r="D387" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E387" t="inlineStr">
         <is>
-          <t>809526162</t>
+          <t>ICD30709299</t>
         </is>
       </c>
       <c r="F387" t="inlineStr">
@@ -29720,7 +29720,7 @@
       </c>
       <c r="H387" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomo </t>
         </is>
       </c>
       <c r="I387" t="n">
@@ -29728,7 +29728,7 @@
       </c>
       <c r="J387" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K387" t="inlineStr">
@@ -29738,18 +29738,18 @@
       </c>
       <c r="L387" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M387" t="n">
-        <v>-58.432726</v>
+        <v>-58.390906</v>
       </c>
       <c r="N387" t="n">
-        <v>-34.582328</v>
+        <v>-34.634312</v>
       </c>
       <c r="O387" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P387" t="inlineStr">
@@ -29761,7 +29761,7 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>7194</t>
+          <t>-586</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
@@ -29771,17 +29771,17 @@
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>CASEROS AV. 2032</t>
+          <t>Franklin 666</t>
         </is>
       </c>
       <c r="D388" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E388" t="inlineStr">
         <is>
-          <t>ICD30709299</t>
+          <t>ICD30709119</t>
         </is>
       </c>
       <c r="F388" t="inlineStr">
@@ -29796,7 +29796,7 @@
       </c>
       <c r="H388" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomo </t>
+          <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
         </is>
       </c>
       <c r="I388" t="n">
@@ -29804,7 +29804,7 @@
       </c>
       <c r="J388" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K388" t="inlineStr">
@@ -29814,18 +29814,18 @@
       </c>
       <c r="L388" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M388" t="n">
-        <v>-58.390906</v>
+        <v>-58.441362</v>
       </c>
       <c r="N388" t="n">
-        <v>-34.634312</v>
+        <v>-34.607784</v>
       </c>
       <c r="O388" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P388" t="inlineStr">
@@ -29837,7 +29837,7 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>-586</t>
+          <t>-587</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
@@ -29847,22 +29847,22 @@
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>Franklin 666</t>
+          <t>ARIAS 4048</t>
         </is>
       </c>
       <c r="D389" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E389" t="inlineStr">
         <is>
-          <t>ICD30709119</t>
+          <t>809526164</t>
         </is>
       </c>
       <c r="F389" t="inlineStr">
         <is>
-          <t>PEBCOM</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G389" t="inlineStr">
@@ -29872,7 +29872,7 @@
       </c>
       <c r="H389" t="inlineStr">
         <is>
-          <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
+          <t>Cambiar 114 picada</t>
         </is>
       </c>
       <c r="I389" t="n">
@@ -29880,7 +29880,7 @@
       </c>
       <c r="J389" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K389" t="inlineStr">
@@ -29894,51 +29894,51 @@
         </is>
       </c>
       <c r="M389" t="n">
-        <v>-58.441362</v>
+        <v>-58.488936</v>
       </c>
       <c r="N389" t="n">
-        <v>-34.607784</v>
+        <v>-34.549005</v>
       </c>
       <c r="O389" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P389" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>-587</t>
+          <t>-588</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>9/8/2025</t>
+          <t>9/9/2025</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>ARIAS 4048</t>
+          <t>Uruguay 259</t>
         </is>
       </c>
       <c r="D390" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E390" t="inlineStr">
         <is>
-          <t>809526164</t>
+          <t>809575010</t>
         </is>
       </c>
       <c r="F390" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>Sin Asignar</t>
         </is>
       </c>
       <c r="G390" t="inlineStr">
@@ -29948,7 +29948,7 @@
       </c>
       <c r="H390" t="inlineStr">
         <is>
-          <t>Cambiar 114 picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I390" t="n">
@@ -29961,7 +29961,7 @@
       </c>
       <c r="K390" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L390" t="inlineStr">
@@ -29970,26 +29970,26 @@
         </is>
       </c>
       <c r="M390" t="n">
-        <v>-58.488936</v>
+        <v>-58.386393</v>
       </c>
       <c r="N390" t="n">
-        <v>-34.549005</v>
+        <v>-34.605812</v>
       </c>
       <c r="O390" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P390" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>-588</t>
+          <t>-589</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
@@ -29999,22 +29999,22 @@
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>Uruguay 259</t>
+          <t>Balbin 4059</t>
         </is>
       </c>
       <c r="D391" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E391" t="inlineStr">
         <is>
-          <t>809575010</t>
+          <t>809575056</t>
         </is>
       </c>
       <c r="F391" t="inlineStr">
         <is>
-          <t>Sin Asignar</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G391" t="inlineStr">
@@ -30024,7 +30024,7 @@
       </c>
       <c r="H391" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Corrimiento ver con Pablo</t>
         </is>
       </c>
       <c r="I391" t="n">
@@ -30037,35 +30037,35 @@
       </c>
       <c r="K391" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L391" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M391" t="n">
-        <v>-58.386393</v>
+        <v>-58.48797</v>
       </c>
       <c r="N391" t="n">
-        <v>-34.605812</v>
+        <v>-34.554733</v>
       </c>
       <c r="O391" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P391" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>-589</t>
+          <t>-590</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
@@ -30075,7 +30075,7 @@
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>Balbin 4059</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D392" t="inlineStr">
@@ -30085,7 +30085,7 @@
       </c>
       <c r="E392" t="inlineStr">
         <is>
-          <t>809575056</t>
+          <t>809575080</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
@@ -30118,14 +30118,14 @@
       </c>
       <c r="L392" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M392" t="n">
-        <v>-58.48797</v>
+        <v>-58.487821</v>
       </c>
       <c r="N392" t="n">
-        <v>-34.554733</v>
+        <v>-34.554603</v>
       </c>
       <c r="O392" t="inlineStr">
         <is>
@@ -30141,7 +30141,7 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>-590</t>
+          <t>-591</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
@@ -30151,22 +30151,22 @@
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Santa Maria de Oro 2730</t>
         </is>
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E393" t="inlineStr">
         <is>
-          <t>809575080</t>
+          <t>809574969</t>
         </is>
       </c>
       <c r="F393" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>Sin Asignar</t>
         </is>
       </c>
       <c r="G393" t="inlineStr">
@@ -30174,11 +30174,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H393" t="inlineStr">
-        <is>
-          <t>Corrimiento ver con Pablo</t>
-        </is>
-      </c>
+      <c r="H393" t="inlineStr"/>
       <c r="I393" t="n">
         <v>1</v>
       </c>
@@ -30189,7 +30185,7 @@
       </c>
       <c r="K393" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente TLC</t>
         </is>
       </c>
       <c r="L393" t="inlineStr">
@@ -30198,89 +30194,17 @@
         </is>
       </c>
       <c r="M393" t="n">
-        <v>-58.487821</v>
+        <v>-58.422406</v>
       </c>
       <c r="N393" t="n">
-        <v>-34.554603</v>
+        <v>-34.577085</v>
       </c>
       <c r="O393" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P393" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="394">
-      <c r="A394" t="inlineStr">
-        <is>
-          <t>-591</t>
-        </is>
-      </c>
-      <c r="B394" t="inlineStr">
-        <is>
-          <t>9/9/2025</t>
-        </is>
-      </c>
-      <c r="C394" t="inlineStr">
-        <is>
-          <t>Santa Maria de Oro 2730</t>
-        </is>
-      </c>
-      <c r="D394" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E394" t="inlineStr">
-        <is>
-          <t>809574969</t>
-        </is>
-      </c>
-      <c r="F394" t="inlineStr">
-        <is>
-          <t>Sin Asignar</t>
-        </is>
-      </c>
-      <c r="G394" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H394" t="inlineStr"/>
-      <c r="I394" t="n">
-        <v>1</v>
-      </c>
-      <c r="J394" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K394" t="inlineStr">
-        <is>
-          <t>Fuente TLC</t>
-        </is>
-      </c>
-      <c r="L394" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M394" t="n">
-        <v>-58.422406</v>
-      </c>
-      <c r="N394" t="n">
-        <v>-34.577085</v>
-      </c>
-      <c r="O394" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P394" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
@@ -30297,7 +30221,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35302,27 +35226,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-560</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Pinzon 1590</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809098712</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -35337,7 +35261,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada mismo caso que 7083</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -35359,10 +35283,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.373506</v>
+        <v>-58.402244</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.63706</v>
+        <v>-34.619401</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -35378,17 +35302,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -35398,7 +35322,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -35413,7 +35337,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada mismo caso que 7083</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -35435,14 +35359,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.402244</v>
+        <v>-58.393882</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.619401</v>
+        <v>-34.604721</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -35454,7 +35378,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -35464,7 +35388,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -35474,7 +35398,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -35511,14 +35435,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.393882</v>
+        <v>-58.394543</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.604721</v>
+        <v>-34.620732</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -35530,7 +35454,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -35540,17 +35464,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -35583,18 +35507,18 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.394543</v>
+        <v>-58.427206</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.620732</v>
+        <v>-34.602914</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -35606,7 +35530,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7050</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -35616,17 +35540,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>PRINGLES 788</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809195664</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -35636,12 +35560,12 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -35654,7 +35578,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
@@ -35663,14 +35587,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.427206</v>
+        <v>-58.435017</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.602914</v>
+        <v>-34.622044</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -35682,17 +35606,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>7064</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>GAONA AV. 1189</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -35702,7 +35626,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809257408</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -35712,12 +35636,12 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -35730,7 +35654,7 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
@@ -35739,14 +35663,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.435017</v>
+        <v>-58.446008</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.622044</v>
+        <v>-34.607602</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -35758,7 +35682,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7064</t>
+          <t>7097</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -35768,17 +35692,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>GAONA AV. 1189</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809257408</t>
+          <t>809279093</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -35793,7 +35717,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -35815,14 +35739,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.446008</v>
+        <v>-58.458659</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.607602</v>
+        <v>-34.630464</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -35834,27 +35758,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7097</t>
+          <t>4698</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
+          <t>REPETTO, NICOLAS, DR. 93</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809279093</t>
+          <t>ICD30593982</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -35864,12 +35788,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -35882,7 +35806,7 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -35891,10 +35815,10 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.458659</v>
+        <v>-58.443232</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.630464</v>
+        <v>-34.620007</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -35910,17 +35834,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>4698</t>
+          <t>7102</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/30/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
+          <t>AMBERES 995</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -35930,7 +35854,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>ICD30593982</t>
+          <t>809309598</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -35940,12 +35864,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -35958,19 +35882,19 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.443232</v>
+        <v>-58.453382</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.620007</v>
+        <v>-34.612707</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -35986,27 +35910,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7102</t>
+          <t>7112</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/30/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>AMBERES 995</t>
+          <t>OLLEROS 2488</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809309598</t>
+          <t>809371829</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -36021,7 +35945,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -36039,18 +35963,18 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.453382</v>
+        <v>-58.444214</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.612707</v>
+        <v>-34.571197</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -36062,27 +35986,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7112</t>
+          <t>7120</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>OLLEROS 2488</t>
+          <t>BLANCO ENCALADA 4210</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809371829</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -36097,7 +36021,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Colocar R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -36110,55 +36034,55 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.444214</v>
+        <v>-58.477593</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.571197</v>
+        <v>-34.570321</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7120</t>
+          <t>7136</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/3/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>BLANCO ENCALADA 4210</t>
+          <t>FERRARI 455</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809427020</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -36173,7 +36097,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir traspaso de fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -36186,23 +36110,23 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.477593</v>
+        <v>-58.441587</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.570321</v>
+        <v>-34.60547</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -36214,7 +36138,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7136</t>
+          <t>7150</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -36224,17 +36148,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>FERRARI 455</t>
+          <t>Bartolomé Mitre 3070</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809427020</t>
+          <t>809427021</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -36249,7 +36173,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -36267,50 +36191,50 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.441587</v>
+        <v>-58.410025</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.60547</v>
+        <v>-34.609184</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7150</t>
+          <t>-585</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>9/3/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Bartolomé Mitre 3070</t>
+          <t>Rio Cuarto 3267</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809427021</t>
+          <t>ICD30704450</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -36325,7 +36249,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Desmonte de columna</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -36333,7 +36257,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -36343,18 +36267,18 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.410025</v>
+        <v>-58.39368</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.609184</v>
+        <v>-34.652663</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -36366,7 +36290,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>-585</t>
+          <t>7180</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -36376,17 +36300,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Rio Cuarto 3267</t>
+          <t>GORRITI 4417</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>ICD30704450</t>
+          <t>809526157</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -36401,7 +36325,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Desmonte de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -36409,7 +36333,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -36419,18 +36343,18 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.39368</v>
+        <v>-58.425358</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.652663</v>
+        <v>-34.593308</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -36442,7 +36366,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7180</t>
+          <t>7186</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -36452,7 +36376,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>GORRITI 4417</t>
+          <t>NICARAGUA 5510</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -36462,7 +36386,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809526157</t>
+          <t>809526162</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -36499,10 +36423,10 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.425358</v>
+        <v>-58.432726</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.593308</v>
+        <v>-34.582328</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -36518,7 +36442,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7186</t>
+          <t>7194</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -36528,17 +36452,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>NICARAGUA 5510</t>
+          <t>CASEROS AV. 2032</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>809526162</t>
+          <t>ICD30709299</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -36553,7 +36477,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomo </t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -36561,7 +36485,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -36571,18 +36495,18 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.432726</v>
+        <v>-58.390906</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.582328</v>
+        <v>-34.634312</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -36594,7 +36518,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7194</t>
+          <t>-586</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -36604,17 +36528,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>CASEROS AV. 2032</t>
+          <t>Franklin 666</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>ICD30709299</t>
+          <t>ICD30709119</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -36629,7 +36553,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomo </t>
+          <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -36637,7 +36561,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -36647,97 +36571,21 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.390906</v>
+        <v>-58.441362</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.634312</v>
+        <v>-34.607784</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>-586</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>9/8/2025</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Franklin 666</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>ICD30709119</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
-        </is>
-      </c>
-      <c r="I85" t="n">
-        <v>1</v>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>Desmonte</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M85" t="n">
-        <v>-58.441362</v>
-      </c>
-      <c r="N85" t="n">
-        <v>-34.607784</v>
-      </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P85" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-16 09:03:58)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P375"/>
+  <dimension ref="A1:P380"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27257,7 +27257,7 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>-580</t>
+          <t>7237</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
@@ -27267,7 +27267,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>Av Nazca 3985</t>
+          <t>NAZCA 3985</t>
         </is>
       </c>
       <c r="D355" t="inlineStr">
@@ -27282,7 +27282,7 @@
       </c>
       <c r="F355" t="inlineStr">
         <is>
-          <t>Sin Asignar</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G355" t="inlineStr">
@@ -28169,32 +28169,32 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>-591</t>
+          <t>-592</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>9/9/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>Santa Maria de Oro 2730</t>
+          <t>VARELA 3018</t>
         </is>
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E367" t="inlineStr">
         <is>
-          <t>809574969</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F367" t="inlineStr">
         <is>
-          <t>Sin Asignar</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G367" t="inlineStr">
@@ -28202,7 +28202,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H367" t="inlineStr"/>
+      <c r="H367" t="inlineStr">
+        <is>
+          <t>Desmonte de columna</t>
+        </is>
+      </c>
       <c r="I367" t="n">
         <v>1</v>
       </c>
@@ -28213,7 +28217,7 @@
       </c>
       <c r="K367" t="inlineStr">
         <is>
-          <t>Fuente TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L367" t="inlineStr">
@@ -28222,14 +28226,14 @@
         </is>
       </c>
       <c r="M367" t="n">
-        <v>-58.422406</v>
+        <v>-58.435989</v>
       </c>
       <c r="N367" t="n">
-        <v>-34.577085</v>
+        <v>-34.657716</v>
       </c>
       <c r="O367" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P367" t="inlineStr">
@@ -28241,7 +28245,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>-592</t>
+          <t>-593</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
@@ -28251,22 +28255,22 @@
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>VARELA 3018</t>
+          <t>Husares 2250</t>
         </is>
       </c>
       <c r="D368" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>809642176</t>
+          <t>809642190</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>Optical Power</t>
         </is>
       </c>
       <c r="G368" t="inlineStr">
@@ -28276,7 +28280,7 @@
       </c>
       <c r="H368" t="inlineStr">
         <is>
-          <t>Corrimiento columna evaluar con Pablo la posicion</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I368" t="n">
@@ -28298,26 +28302,26 @@
         </is>
       </c>
       <c r="M368" t="n">
-        <v>-58.435989</v>
+        <v>-58.443269</v>
       </c>
       <c r="N368" t="n">
-        <v>-34.657716</v>
+        <v>-34.552209</v>
       </c>
       <c r="O368" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P368" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>-593</t>
+          <t>-594</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
@@ -28327,7 +28331,7 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>Husares 2250</t>
+          <t>Vidal 1861</t>
         </is>
       </c>
       <c r="D369" t="inlineStr">
@@ -28337,7 +28341,7 @@
       </c>
       <c r="E369" t="inlineStr">
         <is>
-          <t>809642190</t>
+          <t>809642175</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
@@ -28374,14 +28378,14 @@
         </is>
       </c>
       <c r="M369" t="n">
-        <v>-58.443269</v>
+        <v>-58.458298</v>
       </c>
       <c r="N369" t="n">
-        <v>-34.552209</v>
+        <v>-34.566511</v>
       </c>
       <c r="O369" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P369" t="inlineStr">
@@ -28393,32 +28397,32 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>-594</t>
+          <t>7247</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>9/11/2025</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>Vidal 1861</t>
+          <t>ARAUJO 3430</t>
         </is>
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E370" t="inlineStr">
         <is>
-          <t>809642175</t>
+          <t>809687268</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
         <is>
-          <t>Optical Power</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G370" t="inlineStr">
@@ -28450,51 +28454,51 @@
         </is>
       </c>
       <c r="M370" t="n">
-        <v>-58.458298</v>
+        <v>-58.46866</v>
       </c>
       <c r="N370" t="n">
-        <v>-34.566511</v>
+        <v>-34.669465</v>
       </c>
       <c r="O370" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P370" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>-595</t>
+          <t>-596</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>9/11/2025</t>
+          <t>9/14/2025</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>Araujo 3433</t>
+          <t>Humahuaca 3866</t>
         </is>
       </c>
       <c r="D371" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E371" t="inlineStr">
         <is>
-          <t>809687268</t>
+          <t>809732190</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>Sin Asignar</t>
         </is>
       </c>
       <c r="G371" t="inlineStr">
@@ -28526,14 +28530,14 @@
         </is>
       </c>
       <c r="M371" t="n">
-        <v>-58.469721</v>
+        <v>-58.418823</v>
       </c>
       <c r="N371" t="n">
-        <v>-34.668753</v>
+        <v>-34.602148</v>
       </c>
       <c r="O371" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P371" t="inlineStr">
@@ -28545,32 +28549,32 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>-596</t>
+          <t>7218</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>9/14/2025</t>
+          <t>9/15/2025</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>Humahuaca 3866</t>
+          <t>SAN NICOLAS 5123</t>
         </is>
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E372" t="inlineStr">
         <is>
-          <t>809732190</t>
+          <t>809758863</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
         <is>
-          <t>Sin Asignar</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G372" t="inlineStr">
@@ -28580,7 +28584,7 @@
       </c>
       <c r="H372" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I372" t="n">
@@ -28598,30 +28602,30 @@
       </c>
       <c r="L372" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M372" t="n">
-        <v>-58.418823</v>
+        <v>-58.516218</v>
       </c>
       <c r="N372" t="n">
-        <v>-34.602148</v>
+        <v>-34.589343</v>
       </c>
       <c r="O372" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P372" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>7220</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
@@ -28631,22 +28635,22 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>GUTENBERG 2901</t>
         </is>
       </c>
       <c r="D373" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E373" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>809758870</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
         <is>
-          <t>AYKO</t>
+          <t>NEW</t>
         </is>
       </c>
       <c r="G373" t="inlineStr">
@@ -28656,7 +28660,7 @@
       </c>
       <c r="H373" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I373" t="n">
@@ -28674,14 +28678,14 @@
       </c>
       <c r="L373" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M373" t="n">
-        <v>-58.516218</v>
+        <v>-58.496084</v>
       </c>
       <c r="N373" t="n">
-        <v>-34.589343</v>
+        <v>-34.593316</v>
       </c>
       <c r="O373" t="inlineStr">
         <is>
@@ -28697,7 +28701,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>7220</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -28707,22 +28711,22 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>GUTENBERG 2901</t>
+          <t>SANABRIA 4817</t>
         </is>
       </c>
       <c r="D374" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E374" t="inlineStr">
         <is>
-          <t>809758870</t>
+          <t>809758873</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>AYKO</t>
         </is>
       </c>
       <c r="G374" t="inlineStr">
@@ -28732,7 +28736,7 @@
       </c>
       <c r="H374" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
         </is>
       </c>
       <c r="I374" t="n">
@@ -28754,10 +28758,10 @@
         </is>
       </c>
       <c r="M374" t="n">
-        <v>-58.496084</v>
+        <v>-58.520505</v>
       </c>
       <c r="N374" t="n">
-        <v>-34.593316</v>
+        <v>-34.596045</v>
       </c>
       <c r="O374" t="inlineStr">
         <is>
@@ -28773,76 +28777,456 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>7224</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/16/2025</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>SANABRIA 4817</t>
+          <t>CABILDO AV. 3950</t>
         </is>
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t>809758873</t>
+          <t>809784515</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
         <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G375" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H375" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
+      <c r="I375" t="n">
+        <v>1</v>
+      </c>
+      <c r="J375" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K375" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L375" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M375" t="n">
+        <v>-58.469735</v>
+      </c>
+      <c r="N375" t="n">
+        <v>-34.547232</v>
+      </c>
+      <c r="O375" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P375" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>7225</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>AMENABAR 3590</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>809784519</t>
+        </is>
+      </c>
+      <c r="F376" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G376" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H376" t="inlineStr">
+        <is>
+          <t>Reparar rienda y tambien reclaman columna picada pero no se ve la foto verificarla y evaluar cambio</t>
+        </is>
+      </c>
+      <c r="I376" t="n">
+        <v>1</v>
+      </c>
+      <c r="J376" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K376" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L376" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M376" t="n">
+        <v>-58.470045</v>
+      </c>
+      <c r="N376" t="n">
+        <v>-34.550272</v>
+      </c>
+      <c r="O376" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P376" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>7229</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>AZURDUY JUANA 2627</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
+      <c r="F377" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G377" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H377" t="inlineStr">
+        <is>
+          <t>Colocar columna para pedir traspaso de nodo propio</t>
+        </is>
+      </c>
+      <c r="I377" t="n">
+        <v>1</v>
+      </c>
+      <c r="J377" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K377" t="inlineStr">
+        <is>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L377" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M377" t="n">
+        <v>-58.469008</v>
+      </c>
+      <c r="N377" t="n">
+        <v>-34.552083</v>
+      </c>
+      <c r="O377" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P377" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>7234</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>MOLDES 3388</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>809784522</t>
+        </is>
+      </c>
+      <c r="F378" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G378" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H378" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I378" t="n">
+        <v>1</v>
+      </c>
+      <c r="J378" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K378" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L378" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M378" t="n">
+        <v>-58.469426</v>
+      </c>
+      <c r="N378" t="n">
+        <v>-34.552639</v>
+      </c>
+      <c r="O378" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P378" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>7240</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>LARRALDE, CRISOLOGO AV. 3875</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>809784524</t>
+        </is>
+      </c>
+      <c r="F379" t="inlineStr">
+        <is>
           <t>AYKO</t>
         </is>
       </c>
-      <c r="G375" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H375" t="inlineStr">
-        <is>
-          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
-        </is>
-      </c>
-      <c r="I375" t="n">
-        <v>1</v>
-      </c>
-      <c r="J375" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K375" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L375" t="inlineStr">
+      <c r="G379" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H379" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I379" t="n">
+        <v>1</v>
+      </c>
+      <c r="J379" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K379" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L379" t="inlineStr">
         <is>
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M375" t="n">
-        <v>-58.520505</v>
-      </c>
-      <c r="N375" t="n">
-        <v>-34.596045</v>
-      </c>
-      <c r="O375" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P375" t="inlineStr">
+      <c r="M379" t="n">
+        <v>-58.481316</v>
+      </c>
+      <c r="N379" t="n">
+        <v>-34.556157</v>
+      </c>
+      <c r="O379" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P379" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>7248</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>FERNANDEZ DE LA CRUZ, F., GRAL. AV. 4065</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>809784526</t>
+        </is>
+      </c>
+      <c r="F380" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G380" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Columna chocada </t>
+        </is>
+      </c>
+      <c r="I380" t="n">
+        <v>1</v>
+      </c>
+      <c r="J380" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K380" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L380" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M380" t="n">
+        <v>-58.455155</v>
+      </c>
+      <c r="N380" t="n">
+        <v>-34.669378</v>
+      </c>
+      <c r="O380" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P380" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
@@ -28857,7 +29241,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P79"/>
+  <dimension ref="A1:P82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34844,6 +35228,234 @@
       <c r="P79" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>7224</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>CABILDO AV. 3950</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>809784515</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>1</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
+        <v>-58.469735</v>
+      </c>
+      <c r="N80" t="n">
+        <v>-34.547232</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>7225</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>AMENABAR 3590</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>809784519</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Reparar rienda y tambien reclaman columna picada pero no se ve la foto verificarla y evaluar cambio</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>-58.470045</v>
+      </c>
+      <c r="N81" t="n">
+        <v>-34.550272</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>7234</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>MOLDES 3388</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>809784522</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>-58.469426</v>
+      </c>
+      <c r="N82" t="n">
+        <v>-34.552639</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
@@ -34858,7 +35470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P92"/>
+  <dimension ref="A1:P95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41315,27 +41927,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>7169</t>
+          <t>7237</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>9/5/2025</t>
+          <t>9/3/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5045</t>
+          <t>NAZCA 3985</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>809492980</t>
+          <t>809409491</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -41350,7 +41962,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Poste quebrado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -41368,14 +41980,14 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.515637</v>
+        <v>-58.497366</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.589993</v>
+        <v>-34.591544</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -41391,27 +42003,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>-589</t>
+          <t>7169</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>9/9/2025</t>
+          <t>9/5/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Balbin 4059</t>
+          <t>SAN NICOLAS 5045</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>809575056</t>
+          <t>809492980</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -41426,7 +42038,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Corrimiento ver con Pablo</t>
+          <t>Poste quebrado</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -41444,18 +42056,18 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.48797</v>
+        <v>-58.515637</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.554733</v>
+        <v>-34.589993</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
@@ -41467,7 +42079,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>-590</t>
+          <t>-589</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -41477,7 +42089,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Balbin 4059</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -41487,7 +42099,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>809575080</t>
+          <t>809575056</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -41520,14 +42132,14 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.487821</v>
+        <v>-58.48797</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.554603</v>
+        <v>-34.554733</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
@@ -41543,27 +42155,27 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>-592</t>
+          <t>-590</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>9/9/2025</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>VARELA 3018</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>809642176</t>
+          <t>809575080</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -41578,7 +42190,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Corrimiento columna evaluar con Pablo la posicion</t>
+          <t>Corrimiento ver con Pablo</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -41600,36 +42212,36 @@
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.435989</v>
+        <v>-58.487821</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.657716</v>
+        <v>-34.554603</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>-595</t>
+          <t>-592</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>9/11/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Araujo 3433</t>
+          <t>VARELA 3018</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -41639,7 +42251,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>809687268</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -41654,7 +42266,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmonte de columna</t>
         </is>
       </c>
       <c r="I90" t="n">
@@ -41676,14 +42288,14 @@
         </is>
       </c>
       <c r="M90" t="n">
-        <v>-58.469721</v>
+        <v>-58.435989</v>
       </c>
       <c r="N90" t="n">
-        <v>-34.668753</v>
+        <v>-34.657716</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
@@ -41695,27 +42307,27 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>7247</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/11/2025</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>ARAUJO 3430</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>809687268</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -41730,7 +42342,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I91" t="n">
@@ -41748,99 +42360,327 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M91" t="n">
-        <v>-58.516218</v>
+        <v>-58.46866</v>
       </c>
       <c r="N91" t="n">
-        <v>-34.589343</v>
+        <v>-34.669465</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P91" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
+          <t>7218</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>9/15/2025</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>SAN NICOLAS 5123</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>809758863</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I92" t="n">
+        <v>1</v>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M92" t="n">
+        <v>-58.516218</v>
+      </c>
+      <c r="N92" t="n">
+        <v>-34.589343</v>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P92" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
           <t>2005</t>
         </is>
       </c>
-      <c r="B92" t="inlineStr">
+      <c r="B93" t="inlineStr">
         <is>
           <t>9/15/2025</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr">
+      <c r="C93" t="inlineStr">
         <is>
           <t>SANABRIA 4817</t>
         </is>
       </c>
-      <c r="D92" t="inlineStr">
+      <c r="D93" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr">
+      <c r="E93" t="inlineStr">
         <is>
           <t>809758873</t>
         </is>
       </c>
-      <c r="F92" t="inlineStr">
+      <c r="F93" t="inlineStr">
         <is>
           <t>AYKO</t>
         </is>
       </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
         <is>
           <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
         </is>
       </c>
-      <c r="I92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J92" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L92" t="inlineStr">
+      <c r="I93" t="n">
+        <v>1</v>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
         <is>
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M92" t="n">
+      <c r="M93" t="n">
         <v>-58.520505</v>
       </c>
-      <c r="N92" t="n">
+      <c r="N93" t="n">
         <v>-34.596045</v>
       </c>
-      <c r="O92" t="inlineStr">
+      <c r="O93" t="inlineStr">
         <is>
           <t>Paternal</t>
         </is>
       </c>
-      <c r="P92" t="inlineStr">
+      <c r="P93" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>7240</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>LARRALDE, CRISOLOGO AV. 3875</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>809784524</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I94" t="n">
+        <v>1</v>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M94" t="n">
+        <v>-58.481316</v>
+      </c>
+      <c r="N94" t="n">
+        <v>-34.556157</v>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P94" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>7248</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>FERNANDEZ DE LA CRUZ, F., GRAL. AV. 4065</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>809784526</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Columna chocada </t>
+        </is>
+      </c>
+      <c r="I95" t="n">
+        <v>1</v>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M95" t="n">
+        <v>-58.455155</v>
+      </c>
+      <c r="N95" t="n">
+        <v>-34.669378</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P95" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
@@ -46381,7 +47221,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -48662,27 +49502,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-580</t>
+          <t>-588</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>9/3/2025</t>
+          <t>9/9/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Av Nazca 3985</t>
+          <t>Uruguay 259</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>809409491</t>
+          <t>809575010</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -48710,7 +49550,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -48719,46 +49559,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.497366</v>
+        <v>-58.386393</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.591544</v>
+        <v>-34.605812</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-588</t>
+          <t>-596</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>9/9/2025</t>
+          <t>9/14/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Uruguay 259</t>
+          <t>Humahuaca 3866</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>809575010</t>
+          <t>809732190</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -48786,7 +49626,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -48795,165 +49635,17 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.386393</v>
+        <v>-58.418823</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.605812</v>
+        <v>-34.602148</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>-591</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>9/9/2025</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Santa Maria de Oro 2730</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>809574969</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Sin Asignar</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="n">
-        <v>1</v>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>Fuente TLC</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M33" t="n">
-        <v>-58.422406</v>
-      </c>
-      <c r="N33" t="n">
-        <v>-34.577085</v>
-      </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P33" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>-596</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>9/14/2025</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Humahuaca 3866</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>809732190</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Sin Asignar</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I34" t="n">
-        <v>1</v>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M34" t="n">
-        <v>-58.418823</v>
-      </c>
-      <c r="N34" t="n">
-        <v>-34.602148</v>
-      </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P34" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
@@ -48970,7 +49662,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -54443,6 +55135,82 @@
         </is>
       </c>
       <c r="P72" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>7229</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>AZURDUY JUANA 2627</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>NEW</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Colocar columna para pedir traspaso de nodo propio</t>
+        </is>
+      </c>
+      <c r="I73" t="n">
+        <v>1</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M73" t="n">
+        <v>-58.469008</v>
+      </c>
+      <c r="N73" t="n">
+        <v>-34.552083</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-30 06:56:14)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R380"/>
+  <dimension ref="A1:R384"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -637,7 +637,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>782794907</t>
+          <t>Pendiente de Carga</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -647,10 +647,14 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Desmontar columna ya traspasaron nodo</t>
+        </is>
+      </c>
       <c r="I3" t="n">
         <v>1</v>
       </c>
@@ -33019,6 +33023,350 @@
       <c r="R380" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>-620</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>9/29/2025</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>Luis Viale 3098</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>810056875</t>
+        </is>
+      </c>
+      <c r="F381" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G381" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H381" t="inlineStr">
+        <is>
+          <t>picada</t>
+        </is>
+      </c>
+      <c r="I381" t="n">
+        <v>1</v>
+      </c>
+      <c r="J381" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K381" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L381" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M381" t="n">
+        <v>-58.477413</v>
+      </c>
+      <c r="N381" t="n">
+        <v>-34.620772</v>
+      </c>
+      <c r="O381" t="inlineStr">
+        <is>
+          <t>Devoto</t>
+        </is>
+      </c>
+      <c r="P381" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q381" t="inlineStr">
+        <is>
+          <t>NRA-M</t>
+        </is>
+      </c>
+      <c r="R381" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>-621</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>9/29/2025</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>Tres Arroyos 2911</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>810056868</t>
+        </is>
+      </c>
+      <c r="F382" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G382" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H382" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I382" t="n">
+        <v>1</v>
+      </c>
+      <c r="J382" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K382" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L382" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M382" t="n">
+        <v>-58.476877</v>
+      </c>
+      <c r="N382" t="n">
+        <v>-34.617525</v>
+      </c>
+      <c r="O382" t="inlineStr">
+        <is>
+          <t>Devoto</t>
+        </is>
+      </c>
+      <c r="P382" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q382" t="inlineStr">
+        <is>
+          <t>NRA-M</t>
+        </is>
+      </c>
+      <c r="R382" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>-622</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>9/29/2025</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>Mariano Acha 2271</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>810056867</t>
+        </is>
+      </c>
+      <c r="F383" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G383" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H383" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I383" t="n">
+        <v>1</v>
+      </c>
+      <c r="J383" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K383" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L383" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M383" t="n">
+        <v>-58.477338</v>
+      </c>
+      <c r="N383" t="n">
+        <v>-34.571921</v>
+      </c>
+      <c r="O383" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P383" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q383" t="inlineStr">
+        <is>
+          <t>ATH-J</t>
+        </is>
+      </c>
+      <c r="R383" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>-623</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>9/29/2025</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>Mosconi 3368</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>810061513</t>
+        </is>
+      </c>
+      <c r="F384" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G384" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H384" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I384" t="n">
+        <v>1</v>
+      </c>
+      <c r="J384" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K384" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L384" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M384" t="n">
+        <v>-58.508377</v>
+      </c>
+      <c r="N384" t="n">
+        <v>-34.590137</v>
+      </c>
+      <c r="O384" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P384" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q384" t="inlineStr">
+        <is>
+          <t>PUE-N</t>
+        </is>
+      </c>
+      <c r="R384" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.2PUE</t>
         </is>
       </c>
     </row>
@@ -33238,7 +33586,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>782794907</t>
+          <t>Pendiente de Carga</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -33248,10 +33596,14 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Desmontar columna ya traspasaron nodo</t>
+        </is>
+      </c>
       <c r="I3" t="n">
         <v>1</v>
       </c>
@@ -51555,7 +51907,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R61"/>
+  <dimension ref="A1:R65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -56792,6 +57144,350 @@
       <c r="R61" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>-620</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>9/29/2025</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Luis Viale 3098</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>810056875</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>picada</t>
+        </is>
+      </c>
+      <c r="I62" t="n">
+        <v>1</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M62" t="n">
+        <v>-58.477413</v>
+      </c>
+      <c r="N62" t="n">
+        <v>-34.620772</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>Devoto</t>
+        </is>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>NRA-M</t>
+        </is>
+      </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>-621</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>9/29/2025</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Tres Arroyos 2911</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>810056868</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I63" t="n">
+        <v>1</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M63" t="n">
+        <v>-58.476877</v>
+      </c>
+      <c r="N63" t="n">
+        <v>-34.617525</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>Devoto</t>
+        </is>
+      </c>
+      <c r="P63" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>NRA-M</t>
+        </is>
+      </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>-622</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>9/29/2025</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Mariano Acha 2271</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>810056867</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I64" t="n">
+        <v>1</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M64" t="n">
+        <v>-58.477338</v>
+      </c>
+      <c r="N64" t="n">
+        <v>-34.571921</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>ATH-J</t>
+        </is>
+      </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>-623</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>9/29/2025</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Mosconi 3368</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>810061513</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>1</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M65" t="n">
+        <v>-58.508377</v>
+      </c>
+      <c r="N65" t="n">
+        <v>-34.590137</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>PUE-N</t>
+        </is>
+      </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.2PUE</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-10-08 08:43:24)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -32616,7 +32616,7 @@
       </c>
       <c r="F376" t="inlineStr">
         <is>
-          <t>NEW</t>
+          <t>PEBCOM</t>
         </is>
       </c>
       <c r="G376" t="inlineStr">
@@ -34577,7 +34577,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R93"/>
+  <dimension ref="A1:R94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41950,7 +41950,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>7371</t>
+          <t>-627</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -41960,17 +41960,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>GORRITI 4527</t>
+          <t>Av San Martin 3231</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>810093630</t>
+          <t>810093647</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -41985,7 +41985,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna chocada</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -42007,56 +42007,56 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.426261</v>
+        <v>-58.469321</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.592587</v>
+        <v>-34.601663</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q87" t="inlineStr">
         <is>
-          <t>VCR-D</t>
+          <t>NRA-F</t>
         </is>
       </c>
       <c r="R87" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1NRA</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>7378</t>
+          <t>7371</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>10/1/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>VINCHINA 1518</t>
+          <t>GORRITI 4527</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>810132548</t>
+          <t>810093630</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -42093,24 +42093,24 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.468128</v>
+        <v>-58.426261</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.648117</v>
+        <v>-34.592587</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q88" t="inlineStr">
         <is>
-          <t>PPT-N</t>
+          <t>VCR-D</t>
         </is>
       </c>
       <c r="R88" t="inlineStr">
@@ -42122,7 +42122,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>7382</t>
+          <t>7378</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -42132,17 +42132,17 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>SARMIENTO 1495</t>
+          <t>VINCHINA 1518</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>810132686</t>
+          <t>810132548</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -42179,24 +42179,24 @@
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.387767</v>
+        <v>-58.468128</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.60532</v>
+        <v>-34.648117</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q89" t="inlineStr">
         <is>
-          <t>CEN-E</t>
+          <t>PPT-N</t>
         </is>
       </c>
       <c r="R89" t="inlineStr">
@@ -42208,27 +42208,27 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>7428</t>
+          <t>7382</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>10/6/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>ALBERDI, JUAN BAUTISTA AV. 1536</t>
+          <t>SARMIENTO 1495</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>810244453</t>
+          <t>810132686</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -42243,7 +42243,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Cambiar inclinada casi por caer</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I90" t="n">
@@ -42265,14 +42265,14 @@
         </is>
       </c>
       <c r="M90" t="n">
-        <v>-58.449833</v>
+        <v>-58.387767</v>
       </c>
       <c r="N90" t="n">
-        <v>-34.626444</v>
+        <v>-34.60532</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
@@ -42282,7 +42282,7 @@
       </c>
       <c r="Q90" t="inlineStr">
         <is>
-          <t>PCH-A</t>
+          <t>CEN-E</t>
         </is>
       </c>
       <c r="R90" t="inlineStr">
@@ -42294,7 +42294,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>6404</t>
+          <t>7428</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -42304,17 +42304,17 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>LARREA 320</t>
+          <t>ALBERDI, JUAN BAUTISTA AV. 1536</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>810244454</t>
+          <t>810244453</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -42329,7 +42329,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar inclinada casi por caer</t>
         </is>
       </c>
       <c r="I91" t="n">
@@ -42351,14 +42351,14 @@
         </is>
       </c>
       <c r="M91" t="n">
-        <v>-58.402105</v>
+        <v>-58.449833</v>
       </c>
       <c r="N91" t="n">
-        <v>-34.606071</v>
+        <v>-34.626444</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P91" t="inlineStr">
@@ -42368,7 +42368,7 @@
       </c>
       <c r="Q91" t="inlineStr">
         <is>
-          <t>CLI-D</t>
+          <t>PCH-A</t>
         </is>
       </c>
       <c r="R91" t="inlineStr">
@@ -42380,27 +42380,27 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>7442</t>
+          <t>6404</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>10/7/2025</t>
+          <t>10/6/2025</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1232</t>
+          <t>LARREA 320</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>810255071</t>
+          <t>810244454</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -42415,7 +42415,7 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I92" t="n">
@@ -42437,24 +42437,24 @@
         </is>
       </c>
       <c r="M92" t="n">
-        <v>-58.448466</v>
+        <v>-58.402105</v>
       </c>
       <c r="N92" t="n">
-        <v>-34.56829</v>
+        <v>-34.606071</v>
       </c>
       <c r="O92" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P92" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q92" t="inlineStr">
         <is>
-          <t>COG-D</t>
+          <t>CLI-D</t>
         </is>
       </c>
       <c r="R92" t="inlineStr">
@@ -42466,7 +42466,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>7443</t>
+          <t>7442</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -42476,7 +42476,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1158</t>
+          <t>CABILDO AV. 1232</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -42486,7 +42486,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>810255072</t>
+          <t>810255071</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -42501,7 +42501,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I93" t="n">
@@ -42523,27 +42523,113 @@
         </is>
       </c>
       <c r="M93" t="n">
+        <v>-58.448466</v>
+      </c>
+      <c r="N93" t="n">
+        <v>-34.56829</v>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P93" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>COG-D</t>
+        </is>
+      </c>
+      <c r="R93" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>7443</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>10/7/2025</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>CABILDO AV. 1158</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>810255072</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I94" t="n">
+        <v>1</v>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M94" t="n">
         <v>-58.447751</v>
       </c>
-      <c r="N93" t="n">
+      <c r="N94" t="n">
         <v>-34.568653</v>
       </c>
-      <c r="O93" t="inlineStr">
+      <c r="O94" t="inlineStr">
         <is>
           <t>Colegiales</t>
         </is>
       </c>
-      <c r="P93" t="inlineStr">
+      <c r="P94" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q93" t="inlineStr">
+      <c r="Q94" t="inlineStr">
         <is>
           <t>COG-D</t>
         </is>
       </c>
-      <c r="R93" t="inlineStr">
+      <c r="R94" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>
@@ -59808,7 +59894,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R72"/>
+  <dimension ref="A1:R71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -65665,27 +65751,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-627</t>
+          <t>7381</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>10/1/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Av San Martin 3231</t>
+          <t>HONDURAS 4656</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>810093647</t>
+          <t>810132594</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -65700,7 +65786,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Columna chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -65722,36 +65808,36 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.469321</v>
+        <v>-58.426599</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.601663</v>
+        <v>-34.591132</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>NRA-F</t>
+          <t>VCR-F</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1NRA</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7381</t>
+          <t>7403</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -65761,17 +65847,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>HONDURAS 4656</t>
+          <t>MOLDES 2688</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>810132594</t>
+          <t>810132881</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -65786,7 +65872,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar o desmontar poste ver con inspector</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -65808,24 +65894,24 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.426599</v>
+        <v>-58.463815</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.591132</v>
+        <v>-34.558663</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q70" t="inlineStr">
         <is>
-          <t>VCR-F</t>
+          <t>COG-K</t>
         </is>
       </c>
       <c r="R70" t="inlineStr">
@@ -65837,27 +65923,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7403</t>
+          <t>7411</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>10/6/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>MOLDES 2688</t>
+          <t>MERCEDES 3774</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>810132881</t>
+          <t>810244452</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -65872,7 +65958,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Cambiar o desmontar poste ver con inspector</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -65890,18 +65976,18 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.463815</v>
+        <v>-58.511139</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.558663</v>
+        <v>-34.602167</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -65911,96 +65997,10 @@
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>COG-K</t>
+          <t>PUE-P</t>
         </is>
       </c>
       <c r="R71" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>7411</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>10/6/2025</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>MERCEDES 3774</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>810244452</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>NEW</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>Poste inclinado</t>
-        </is>
-      </c>
-      <c r="I72" t="n">
-        <v>1</v>
-      </c>
-      <c r="J72" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M72" t="n">
-        <v>-58.511139</v>
-      </c>
-      <c r="N72" t="n">
-        <v>-34.602167</v>
-      </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P72" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q72" t="inlineStr">
-        <is>
-          <t>PUE-P</t>
-        </is>
-      </c>
-      <c r="R72" t="inlineStr">
         <is>
           <t>ARATO-25058.PO.1PUE</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-17 20:17:42)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="General" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PEBCOM" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Optical_Power" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Propio" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sin_Asignar" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NEW" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AYKO" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="INCO" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="General" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="PEBCOM" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Optical_Power" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Propio" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sin_Asignar" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="NEW" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="AYKO" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="INCO" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-31 06:39:11)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R436"/>
+  <dimension ref="A1:R438"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37841,6 +37841,178 @@
         </is>
       </c>
       <c r="R436" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>-662</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>10/30/2025</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>ARIAS 2941</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E437" t="inlineStr">
+        <is>
+          <t>810490637</t>
+        </is>
+      </c>
+      <c r="F437" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G437" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H437" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I437" t="n">
+        <v>1</v>
+      </c>
+      <c r="J437" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K437" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L437" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M437" t="n">
+        <v>-58.478491</v>
+      </c>
+      <c r="N437" t="n">
+        <v>-34.543969</v>
+      </c>
+      <c r="O437" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P437" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q437" t="inlineStr">
+        <is>
+          <t>COG-P</t>
+        </is>
+      </c>
+      <c r="R437" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>-663</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>10/30/2025</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>ALBERDI, JUAN BAUTISTA AV. 2693</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G438" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H438" t="inlineStr">
+        <is>
+          <t>Picada con nodo teco</t>
+        </is>
+      </c>
+      <c r="I438" t="n">
+        <v>1</v>
+      </c>
+      <c r="J438" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K438" t="inlineStr">
+        <is>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L438" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M438" t="n">
+        <v>-58.465679</v>
+      </c>
+      <c r="N438" t="n">
+        <v>-34.63241</v>
+      </c>
+      <c r="O438" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P438" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q438" t="inlineStr">
+        <is>
+          <t>PCH-H</t>
+        </is>
+      </c>
+      <c r="R438" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>
@@ -54912,7 +55084,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R89"/>
+  <dimension ref="A1:R91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -62555,6 +62727,178 @@
         </is>
       </c>
       <c r="R89" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>-662</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>10/30/2025</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>ARIAS 2941</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>810490637</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M90" t="n">
+        <v>-58.478491</v>
+      </c>
+      <c r="N90" t="n">
+        <v>-34.543969</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>COG-P</t>
+        </is>
+      </c>
+      <c r="R90" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>-663</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>10/30/2025</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>ALBERDI, JUAN BAUTISTA AV. 2693</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Picada con nodo teco</t>
+        </is>
+      </c>
+      <c r="I91" t="n">
+        <v>1</v>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M91" t="n">
+        <v>-58.465679</v>
+      </c>
+      <c r="N91" t="n">
+        <v>-34.63241</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>PCH-H</t>
+        </is>
+      </c>
+      <c r="R91" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-03 07:26:47)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R436"/>
+  <dimension ref="A1:R438"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37763,32 +37763,32 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>-664</t>
+          <t>-665</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>10/31/2025</t>
+          <t>11/2/2025</t>
         </is>
       </c>
       <c r="C436" t="inlineStr">
         <is>
-          <t>Mercedes 346</t>
+          <t>BEIRO, FRANCISCO AV. 3926</t>
         </is>
       </c>
       <c r="D436" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E436" t="inlineStr">
         <is>
-          <t>810493536</t>
+          <t>810526256</t>
         </is>
       </c>
       <c r="F436" t="inlineStr">
         <is>
-          <t>Optical Power</t>
+          <t>Sin Asignar</t>
         </is>
       </c>
       <c r="G436" t="inlineStr">
@@ -37798,11 +37798,11 @@
       </c>
       <c r="H436" t="inlineStr">
         <is>
-          <t>Estaba chocada pasada por Juli</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I436" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J436" t="inlineStr">
         <is>
@@ -37820,10 +37820,10 @@
         </is>
       </c>
       <c r="M436" t="n">
-        <v>-58.484683</v>
+        <v>-58.507687</v>
       </c>
       <c r="N436" t="n">
-        <v>-34.630456</v>
+        <v>-34.603386</v>
       </c>
       <c r="O436" t="inlineStr">
         <is>
@@ -37837,12 +37837,184 @@
       </c>
       <c r="Q436" t="inlineStr">
         <is>
-          <t>DEV-L</t>
+          <t>DEV-C</t>
         </is>
       </c>
       <c r="R436" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2DEV</t>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>-666</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>11/2/2025</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>ALBERDI, JUAN BAUTISTA AV. 2331</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E437" t="inlineStr">
+        <is>
+          <t>810526265</t>
+        </is>
+      </c>
+      <c r="F437" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G437" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H437" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I437" t="n">
+        <v>1</v>
+      </c>
+      <c r="J437" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K437" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L437" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M437" t="n">
+        <v>-58.460681</v>
+      </c>
+      <c r="N437" t="n">
+        <v>-34.63089</v>
+      </c>
+      <c r="O437" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P437" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q437" t="inlineStr">
+        <is>
+          <t>PCH-J</t>
+        </is>
+      </c>
+      <c r="R437" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>-667</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>11/2/2025</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>ALBERDI, JUAN BAUTISTA AV. 2309</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>810526272</t>
+        </is>
+      </c>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G438" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H438" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I438" t="n">
+        <v>1</v>
+      </c>
+      <c r="J438" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K438" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L438" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M438" t="n">
+        <v>-58.460356</v>
+      </c>
+      <c r="N438" t="n">
+        <v>-34.630793</v>
+      </c>
+      <c r="O438" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P438" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q438" t="inlineStr">
+        <is>
+          <t>PCH-J</t>
+        </is>
+      </c>
+      <c r="R438" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -46364,7 +46536,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R96"/>
+  <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -54529,92 +54701,6 @@
       <c r="R95" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>-664</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>10/31/2025</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>Mercedes 346</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>810493536</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>Estaba chocada pasada por Juli</t>
-        </is>
-      </c>
-      <c r="I96" t="n">
-        <v>0</v>
-      </c>
-      <c r="J96" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M96" t="n">
-        <v>-58.484683</v>
-      </c>
-      <c r="N96" t="n">
-        <v>-34.630456</v>
-      </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>Devoto</t>
-        </is>
-      </c>
-      <c r="P96" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q96" t="inlineStr">
-        <is>
-          <t>DEV-L</t>
-        </is>
-      </c>
-      <c r="R96" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>
@@ -54826,7 +54912,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R90"/>
+  <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -62555,6 +62641,264 @@
         </is>
       </c>
       <c r="R90" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>-665</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>11/2/2025</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>BEIRO, FRANCISCO AV. 3926</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>810526256</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I91" t="n">
+        <v>1</v>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M91" t="n">
+        <v>-58.507687</v>
+      </c>
+      <c r="N91" t="n">
+        <v>-34.603386</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>Devoto</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>DEV-C</t>
+        </is>
+      </c>
+      <c r="R91" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>-666</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>11/2/2025</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>ALBERDI, JUAN BAUTISTA AV. 2331</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>810526265</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I92" t="n">
+        <v>1</v>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M92" t="n">
+        <v>-58.460681</v>
+      </c>
+      <c r="N92" t="n">
+        <v>-34.63089</v>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P92" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>PCH-J</t>
+        </is>
+      </c>
+      <c r="R92" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>-667</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>11/2/2025</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>ALBERDI, JUAN BAUTISTA AV. 2309</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>810526272</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Sin Asignar</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I93" t="n">
+        <v>1</v>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M93" t="n">
+        <v>-58.460356</v>
+      </c>
+      <c r="N93" t="n">
+        <v>-34.630793</v>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P93" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>PCH-J</t>
+        </is>
+      </c>
+      <c r="R93" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-06 10:02:14)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="General" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="PEBCOM" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Optical_Power" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Propio" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Sin_Asignar" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="NEW" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="AYKO" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="INCO" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="General" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PEBCOM" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Optical_Power" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Propio" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sin_Asignar" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NEW" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AYKO" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="INCO" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-18 10:58:44)
</commit_message>
<xml_diff>
--- a/mapa_interactivo.xlsx
+++ b/mapa_interactivo.xlsx
@@ -555,7 +555,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787648</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -631,7 +631,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Baunes 2195</t>
+          <t>Bauness 2195</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787633</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -664,7 +664,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -727,7 +727,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787625</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -750,7 +750,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -813,7 +813,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787612</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787606</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -985,7 +985,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787554</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787548</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1157,7 +1157,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787513</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ARCAMENDIA 793</t>
+          <t xml:space="preserve"> ARCAMENDIA 793</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787479</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -37472,7 +37472,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787648</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -37558,7 +37558,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787612</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -37644,7 +37644,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787606</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -37730,7 +37730,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787554</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -37816,7 +37816,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787548</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -37902,7 +37902,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787513</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -37978,7 +37978,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ARCAMENDIA 793</t>
+          <t xml:space="preserve"> ARCAMENDIA 793</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -37988,7 +37988,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787479</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -46919,7 +46919,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Baunes 2195</t>
+          <t>Bauness 2195</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -46929,7 +46929,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787633</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -46952,7 +46952,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -47015,7 +47015,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810787625</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -47038,7 +47038,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">

</xml_diff>